<commit_message>
Some changes for Control version.xls
</commit_message>
<xml_diff>
--- a/1 четверть_3_Введение в контроль версий.xlsx
+++ b/1 четверть_3_Введение в контроль версий.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Desktop\Homework-repo\GB_Developer_Workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D672DE0-51AD-4A70-BD33-067D41C110D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B89567-1CEF-477A-8C28-14066F0C2D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="212">
   <si>
     <t>Урок 1</t>
   </si>
@@ -1950,7 +1950,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1990,6 +1990,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2087,7 +2093,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2174,6 +2180,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3083,8 +3092,8 @@
   </sheetPr>
   <dimension ref="A1:X72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D58" sqref="A58:D61"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3994,9 +4003,7 @@
       <c r="X52" s="3"/>
     </row>
     <row r="53" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A53" s="3" t="s">
-        <v>163</v>
-      </c>
+      <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="C53" s="6"/>
       <c r="F53" s="3"/>
@@ -4016,8 +4023,8 @@
       <c r="X53" s="3"/>
     </row>
     <row r="54" spans="1:24" ht="29" x14ac:dyDescent="0.35">
-      <c r="A54" s="8" t="s">
-        <v>2</v>
+      <c r="A54" s="30" t="s">
+        <v>163</v>
       </c>
       <c r="C54" s="17" t="s">
         <v>174</v>

</xml_diff>

<commit_message>
save 06 11 2025
</commit_message>
<xml_diff>
--- a/1 четверть_3_Введение в контроль версий.xlsx
+++ b/1 четверть_3_Введение в контроль версий.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlexServHW\Desktop\GB_Developer_Workbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63321783-4311-4C0E-840A-FDC8062E08F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A08B6EBC-C5CB-4F6D-86A9-4310953B7535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="684" yWindow="0" windowWidth="22356" windowHeight="16212" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1-3" sheetId="2" r:id="rId1"/>
@@ -21,12 +21,15 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="542">
   <si>
     <t>Урок 1</t>
   </si>
@@ -4717,6 +4720,97 @@
   <si>
     <t>Вывести список веток
 Переименуйте ветку локально</t>
+  </si>
+  <si>
+    <t>git fetch --prune</t>
+  </si>
+  <si>
+    <r>
+      <t>Пример
+$ git branch -a
+  remotes</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/origin/HEAD -&gt; origin/master</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+  remotes</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/origin/Tauri</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+  remotes</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/origin/auth_service</t>
+    </r>
+  </si>
+  <si>
+    <t>git branch | grep 'test_an' | xargs git branch -D</t>
+  </si>
+  <si>
+    <t>Удалить сразу несколько веток локального репозитория</t>
+  </si>
+  <si>
+    <t>git branch -r | grep 'origin/feature/' | sed 's/origin\///' | xargs -I {} git push origin --delete {}</t>
+  </si>
+  <si>
+    <t>Удалить сразу несколько веток удалённого репозитория</t>
+  </si>
+  <si>
+    <t>sed - это команда замены (substitution) в sed. 
+Синтаксис: s/что_заменить/на_что_заменить/
+sed 's/origin\///' заменить подстроку origin/ на пустую строку (то есть просто удалить origin/ из начала строки).
+Обратный слэш \ перед / нужен для **экранирования** символа /, потому что он сам используется как разделитель в команде s/.../.../.</t>
+  </si>
+  <si>
+    <t>Удалить локальные ветки удалённого репозитория
+git branch -r - показать локальные ветки удалённого репозитория
+git branch -a - ВСЕ ветки</t>
   </si>
 </sst>
 </file>
@@ -5543,13 +5637,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>768413</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>145144</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>2202690</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>1415143</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -5587,13 +5681,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>750169</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>2341426</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>1143000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -5631,13 +5725,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>1102741</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>70098</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>1610591</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>785091</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -5675,13 +5769,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>163286</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>263071</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>1989507</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>878744</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -5719,13 +5813,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>785091</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>92365</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>2676097</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>788311</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -5763,13 +5857,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>461798</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>57728</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>1801091</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>806097</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -5807,13 +5901,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>940660</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>70716</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>1492250</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>876885</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -5851,13 +5945,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>196273</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>92363</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>3221182</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>655226</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -5895,13 +5989,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>100514</xdr:colOff>
-      <xdr:row>68</xdr:row>
+      <xdr:row>72</xdr:row>
       <xdr:rowOff>77423</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>3310150</xdr:colOff>
-      <xdr:row>68</xdr:row>
+      <xdr:row>72</xdr:row>
       <xdr:rowOff>378584</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -5939,13 +6033,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>92364</xdr:colOff>
-      <xdr:row>71</xdr:row>
+      <xdr:row>75</xdr:row>
       <xdr:rowOff>103909</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>3425305</xdr:colOff>
-      <xdr:row>71</xdr:row>
+      <xdr:row>75</xdr:row>
       <xdr:rowOff>308118</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -5983,13 +6077,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1373911</xdr:colOff>
-      <xdr:row>72</xdr:row>
+      <xdr:row>76</xdr:row>
       <xdr:rowOff>374210</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>3394365</xdr:colOff>
-      <xdr:row>72</xdr:row>
+      <xdr:row>76</xdr:row>
       <xdr:rowOff>556875</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -6027,13 +6121,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>69272</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>150092</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>3043646</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>1154546</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -6071,13 +6165,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1890059</xdr:colOff>
-      <xdr:row>73</xdr:row>
+      <xdr:row>77</xdr:row>
       <xdr:rowOff>119529</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>3380442</xdr:colOff>
-      <xdr:row>73</xdr:row>
+      <xdr:row>77</xdr:row>
       <xdr:rowOff>657411</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -6115,13 +6209,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1882589</xdr:colOff>
-      <xdr:row>74</xdr:row>
+      <xdr:row>78</xdr:row>
       <xdr:rowOff>134470</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>3309471</xdr:colOff>
-      <xdr:row>74</xdr:row>
+      <xdr:row>78</xdr:row>
       <xdr:rowOff>845831</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -6159,13 +6253,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>190498</xdr:colOff>
-      <xdr:row>73</xdr:row>
+      <xdr:row>77</xdr:row>
       <xdr:rowOff>697311</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>3862613</xdr:colOff>
-      <xdr:row>76</xdr:row>
+      <xdr:row>80</xdr:row>
       <xdr:rowOff>1647612</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -6203,13 +6297,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>118564</xdr:colOff>
-      <xdr:row>76</xdr:row>
+      <xdr:row>80</xdr:row>
       <xdr:rowOff>612054</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1415150</xdr:colOff>
-      <xdr:row>76</xdr:row>
+      <xdr:row>80</xdr:row>
       <xdr:rowOff>1015465</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -6247,13 +6341,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>114195</xdr:colOff>
-      <xdr:row>76</xdr:row>
+      <xdr:row>80</xdr:row>
       <xdr:rowOff>1030408</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1563489</xdr:colOff>
-      <xdr:row>76</xdr:row>
+      <xdr:row>80</xdr:row>
       <xdr:rowOff>1163090</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -6291,13 +6385,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>114193</xdr:colOff>
-      <xdr:row>76</xdr:row>
+      <xdr:row>80</xdr:row>
       <xdr:rowOff>1173159</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1542143</xdr:colOff>
-      <xdr:row>76</xdr:row>
+      <xdr:row>80</xdr:row>
       <xdr:rowOff>1561687</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -6335,7 +6429,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>208110</xdr:colOff>
-      <xdr:row>164</xdr:row>
+      <xdr:row>168</xdr:row>
       <xdr:rowOff>91248</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3119727" cy="1051752"/>
@@ -6374,13 +6468,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>343647</xdr:colOff>
-      <xdr:row>240</xdr:row>
+      <xdr:row>244</xdr:row>
       <xdr:rowOff>622432</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2917952</xdr:colOff>
-      <xdr:row>240</xdr:row>
+      <xdr:row>244</xdr:row>
       <xdr:rowOff>2057948</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -6418,13 +6512,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>358588</xdr:colOff>
-      <xdr:row>243</xdr:row>
+      <xdr:row>247</xdr:row>
       <xdr:rowOff>91490</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2687132</xdr:colOff>
-      <xdr:row>244</xdr:row>
+      <xdr:row>248</xdr:row>
       <xdr:rowOff>4934</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -6462,13 +6556,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>74706</xdr:colOff>
-      <xdr:row>244</xdr:row>
+      <xdr:row>248</xdr:row>
       <xdr:rowOff>138965</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2756856</xdr:colOff>
-      <xdr:row>244</xdr:row>
+      <xdr:row>248</xdr:row>
       <xdr:rowOff>1249542</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -6506,13 +6600,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>500530</xdr:colOff>
-      <xdr:row>115</xdr:row>
+      <xdr:row>119</xdr:row>
       <xdr:rowOff>173012</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>2265472</xdr:colOff>
-      <xdr:row>117</xdr:row>
+      <xdr:row>121</xdr:row>
       <xdr:rowOff>470085</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -6815,10 +6909,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:X271"/>
+  <dimension ref="A1:X275"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="H15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6834,7 +6928,7 @@
     <col min="9" max="9" width="43.5546875" style="5" customWidth="1"/>
     <col min="10" max="10" width="8.77734375" style="2"/>
     <col min="11" max="11" width="39.21875" style="5" customWidth="1"/>
-    <col min="12" max="12" width="40.21875" style="5" customWidth="1"/>
+    <col min="12" max="12" width="44" style="5" customWidth="1"/>
     <col min="13" max="13" width="58.6640625" style="5" customWidth="1"/>
     <col min="14" max="14" width="49.77734375" style="5" customWidth="1"/>
     <col min="15" max="15" width="8.77734375" style="2"/>
@@ -7153,2446 +7247,2476 @@
         <v>528</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
-      <c r="S17" s="1"/>
-      <c r="U17" s="1"/>
-      <c r="V17" s="3"/>
-      <c r="W17" s="3"/>
-      <c r="X17" s="3"/>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+    <row r="17" spans="1:24" ht="72" x14ac:dyDescent="0.3">
+      <c r="K17" s="5" t="s">
+        <v>534</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>535</v>
+      </c>
+      <c r="M17" s="5" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="K18" s="5" t="s">
+        <v>536</v>
+      </c>
+      <c r="M18" s="5" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" ht="144" x14ac:dyDescent="0.3">
+      <c r="K19" s="5" t="s">
+        <v>538</v>
+      </c>
+      <c r="L19" s="5" t="s">
+        <v>540</v>
+      </c>
+      <c r="M19" s="5" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="3"/>
+      <c r="W21" s="3"/>
+      <c r="X21" s="3"/>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="6"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="3"/>
-      <c r="S18" s="3"/>
-      <c r="U18" s="3"/>
-      <c r="V18" s="3"/>
-      <c r="W18" s="3"/>
-      <c r="X18" s="3"/>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A19" s="8" t="s">
+      <c r="B22" s="3"/>
+      <c r="C22" s="6"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="3"/>
+      <c r="U22" s="3"/>
+      <c r="V22" s="3"/>
+      <c r="W22" s="3"/>
+      <c r="X22" s="3"/>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A23" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="5"/>
-      <c r="K19" s="8" t="s">
+      <c r="D23" s="5"/>
+      <c r="K23" s="8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:24" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="10" t="s">
+    <row r="24" spans="1:24" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A24" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C24" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D24" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F24" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="K20" s="5" t="s">
+      <c r="K24" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="L20" s="5" t="s">
+      <c r="L24" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="M20" s="5" t="s">
+      <c r="M24" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="N20" s="9">
+      <c r="N24" s="9">
         <v>2.6041666666666668E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:24" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
+    <row r="25" spans="1:24" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
         <v>532</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B25" s="5" t="s">
         <v>318</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C25" s="5" t="s">
         <v>533</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D25" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F25" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="K21" s="5" t="s">
+      <c r="K25" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="L21" s="5" t="s">
+      <c r="L25" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="M21" s="5" t="s">
+      <c r="M25" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="N21" s="9">
+      <c r="N25" s="9">
         <v>3.0902777777777779E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A22" s="5" t="s">
+    <row r="26" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C26" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D26" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="F26" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="G26" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="H22" s="5" t="s">
+      <c r="H26" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="I22" s="3" t="s">
+      <c r="I26" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="K22" s="5" t="s">
+      <c r="K26" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="L22" s="5" t="s">
+      <c r="L26" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="M22" s="5" t="s">
+      <c r="M26" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="N22" s="9">
+      <c r="N26" s="9">
         <v>5.347222222222222E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:24" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
+    <row r="27" spans="1:24" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C27" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D27" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F27" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="K23" s="5" t="s">
+      <c r="K27" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="L23" s="5" t="s">
+      <c r="L27" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="M23" s="5" t="s">
+      <c r="M27" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="N23" s="9" t="s">
+      <c r="N27" s="9" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:24" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="5" t="s">
+    <row r="28" spans="1:24" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B28" s="12" t="s">
         <v>268</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C28" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D28" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="F28" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="L24" s="13" t="s">
+      <c r="L28" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="M24" s="5" t="s">
+      <c r="M28" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A25" s="10" t="s">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A29" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="K25" s="5" t="s">
+      <c r="K29" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="L25" s="13"/>
-      <c r="M25" s="5" t="s">
+      <c r="L29" s="13"/>
+      <c r="M29" s="5" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="26" spans="1:24" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
+    <row r="30" spans="1:24" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B30" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C30" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D30" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="F30" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="K26" s="5" t="s">
+      <c r="K30" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="L26" s="5" t="s">
+      <c r="L30" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="M26" s="5" t="s">
+      <c r="M30" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="N26" s="9">
+      <c r="N30" s="9">
         <v>9.5138888888888884E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="F27" s="5" t="s">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="F31" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
-      <c r="P29" s="1"/>
-      <c r="Q29" s="1"/>
-      <c r="R29" s="1"/>
-      <c r="S29" s="1"/>
-      <c r="U29" s="1"/>
-      <c r="V29" s="3"/>
-      <c r="W29" s="3"/>
-      <c r="X29" s="3"/>
-    </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1"/>
+      <c r="S33" s="1"/>
+      <c r="U33" s="1"/>
+      <c r="V33" s="3"/>
+      <c r="W33" s="3"/>
+      <c r="X33" s="3"/>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B30" s="3"/>
-      <c r="C30" s="6"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
-      <c r="Q30" s="3"/>
-      <c r="R30" s="3"/>
-      <c r="S30" s="3"/>
-      <c r="U30" s="3"/>
-      <c r="V30" s="3"/>
-      <c r="W30" s="3"/>
-      <c r="X30" s="3"/>
-    </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A31" s="8" t="s">
+      <c r="B34" s="3"/>
+      <c r="C34" s="6"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
+      <c r="Q34" s="3"/>
+      <c r="R34" s="3"/>
+      <c r="S34" s="3"/>
+      <c r="U34" s="3"/>
+      <c r="V34" s="3"/>
+      <c r="W34" s="3"/>
+      <c r="X34" s="3"/>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A35" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D31" s="5"/>
-      <c r="K31" s="8" t="s">
+      <c r="D35" s="5"/>
+      <c r="K35" s="8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A32" s="5" t="s">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D36" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="K32" s="5" t="s">
+      <c r="K36" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="N32" s="9">
+      <c r="N36" s="9">
         <v>5.8333333333333327E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="10" t="s">
+    <row r="37" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="K33" s="5" t="s">
+      <c r="K37" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="N33" s="9">
+      <c r="N37" s="9">
         <v>6.3888888888888884E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A34" s="5" t="s">
+    <row r="38" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C38" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="K34" s="10" t="s">
+      <c r="K38" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="M34" s="14" t="s">
+      <c r="M38" s="14" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="87" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="5" t="s">
+    <row r="39" spans="1:24" ht="87" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B35" s="12" t="s">
+      <c r="B39" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C39" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D39" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="K35" s="5" t="s">
+      <c r="K39" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="L35" s="12" t="s">
+      <c r="L39" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="M35" s="5" t="s">
+      <c r="M39" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="N35" s="9">
+      <c r="N39" s="9">
         <v>6.805555555555555E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A36" s="10" t="s">
+    <row r="40" spans="1:24" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A40" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="K36" s="5" t="s">
+      <c r="K40" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="M36" s="5" t="s">
+      <c r="M40" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="N36" s="9">
+      <c r="N40" s="9">
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="72" x14ac:dyDescent="0.3">
-      <c r="A37" s="5" t="s">
+    <row r="41" spans="1:24" ht="72" x14ac:dyDescent="0.3">
+      <c r="A41" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B37" s="12" t="s">
+      <c r="B41" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C41" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D41" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="L37" s="12" t="s">
+      <c r="L41" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="N37" s="9">
+      <c r="N41" s="9">
         <v>7.5694444444444439E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A38" s="5" t="s">
+    <row r="42" spans="1:24" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A42" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B42" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C42" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D42" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="K38" s="10" t="s">
+      <c r="K42" s="10" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="72" x14ac:dyDescent="0.3">
-      <c r="A39" s="5" t="s">
+    <row r="43" spans="1:24" ht="72" x14ac:dyDescent="0.3">
+      <c r="A43" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B39" s="12" t="s">
+      <c r="B43" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C43" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="K39" s="5" t="s">
+      <c r="K43" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="M39" s="5" t="s">
+      <c r="M43" s="5" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="72" x14ac:dyDescent="0.3">
-      <c r="A40" s="5" t="s">
+    <row r="44" spans="1:24" ht="72" x14ac:dyDescent="0.3">
+      <c r="A44" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="B40" s="12" t="s">
+      <c r="B44" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D44" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="K40" s="10" t="s">
+      <c r="K44" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="M40" s="5" t="s">
+      <c r="M44" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="N40" s="9" t="s">
+      <c r="N44" s="9" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A41" s="10" t="s">
+    <row r="45" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A45" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="K41" s="10" t="s">
+      <c r="K45" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="L41" s="12" t="s">
+      <c r="L45" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="M41" s="5" t="s">
+      <c r="M45" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="N41" s="9">
+      <c r="N45" s="9">
         <v>9.7222222222222224E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A42" s="5" t="s">
+    <row r="46" spans="1:24" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A46" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B42" s="15" t="s">
+      <c r="B46" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C46" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D46" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="K42" s="10" t="s">
+      <c r="K46" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="M42" s="5" t="s">
+      <c r="M46" s="5" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A43" s="5" t="s">
+    <row r="47" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A47" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C47" s="5" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A44" s="5" t="s">
+    <row r="48" spans="1:24" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A48" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B44" s="15" t="s">
+      <c r="B48" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C48" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D48" s="3" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A45" s="5" t="s">
+    <row r="49" spans="1:24" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A49" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="B45" s="12"/>
-      <c r="C45" s="5" t="s">
+      <c r="B49" s="12"/>
+      <c r="C49" s="5" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A46" s="5" t="s">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A50" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="B46" s="12"/>
-      <c r="C46" s="5" t="s">
+      <c r="B50" s="12"/>
+      <c r="C50" s="5" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A47" s="10" t="s">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A51" s="10" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A48" s="5" t="s">
+    <row r="52" spans="1:24" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A52" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="C52" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D52" s="3" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="49" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A49" s="5" t="s">
+    <row r="53" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A53" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B49" s="12" t="s">
+      <c r="B53" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="C53" s="5" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="50" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A50" s="5" t="s">
+    <row r="54" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A54" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="C50" s="5" t="s">
+      <c r="C54" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="D54" s="3" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="51" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A51" s="5" t="s">
+    <row r="55" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A55" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="C51" s="5" t="s">
+      <c r="C55" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="D55" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="52" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A52" s="5" t="s">
+    <row r="56" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A56" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C52" s="5" t="s">
+      <c r="C56" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="D56" s="3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="7"/>
-      <c r="D54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
-      <c r="I54" s="1"/>
-      <c r="K54" s="1"/>
-      <c r="L54" s="1"/>
-      <c r="M54" s="1"/>
-      <c r="N54" s="1"/>
-      <c r="P54" s="1"/>
-      <c r="Q54" s="1"/>
-      <c r="R54" s="1"/>
-      <c r="S54" s="1"/>
-      <c r="U54" s="1"/>
-      <c r="V54" s="3"/>
-      <c r="W54" s="3"/>
-      <c r="X54" s="3"/>
-    </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A55" s="3" t="s">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="7"/>
+      <c r="D58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+      <c r="K58" s="1"/>
+      <c r="L58" s="1"/>
+      <c r="M58" s="1"/>
+      <c r="N58" s="1"/>
+      <c r="P58" s="1"/>
+      <c r="Q58" s="1"/>
+      <c r="R58" s="1"/>
+      <c r="S58" s="1"/>
+      <c r="U58" s="1"/>
+      <c r="V58" s="3"/>
+      <c r="W58" s="3"/>
+      <c r="X58" s="3"/>
+    </row>
+    <row r="59" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A59" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="B55" s="3"/>
-      <c r="C55" s="6"/>
-      <c r="F55" s="3"/>
-      <c r="G55" s="3"/>
-      <c r="H55" s="3"/>
-      <c r="I55" s="3"/>
-      <c r="K55" s="3"/>
-      <c r="L55" s="3"/>
-      <c r="M55" s="3"/>
-      <c r="N55" s="3"/>
-      <c r="Q55" s="3"/>
-      <c r="R55" s="3"/>
-      <c r="S55" s="3"/>
-      <c r="U55" s="3"/>
-      <c r="V55" s="3"/>
-      <c r="W55" s="3"/>
-      <c r="X55" s="3"/>
-    </row>
-    <row r="56" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A56" s="8" t="s">
+      <c r="B59" s="3"/>
+      <c r="C59" s="6"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="3"/>
+      <c r="I59" s="3"/>
+      <c r="K59" s="3"/>
+      <c r="L59" s="3"/>
+      <c r="M59" s="3"/>
+      <c r="N59" s="3"/>
+      <c r="Q59" s="3"/>
+      <c r="R59" s="3"/>
+      <c r="S59" s="3"/>
+      <c r="U59" s="3"/>
+      <c r="V59" s="3"/>
+      <c r="W59" s="3"/>
+      <c r="X59" s="3"/>
+    </row>
+    <row r="60" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A60" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="C56" s="16" t="s">
+      <c r="C60" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="D56" s="5"/>
-      <c r="K56" s="8" t="s">
+      <c r="D60" s="5"/>
+      <c r="K60" s="8" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A57" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A58" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A59" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="60" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A60" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="61" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="62" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A62" s="10" t="s">
-        <v>166</v>
+      <c r="A62" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="63" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="64" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A64" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="10" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="C63" s="5" t="s">
+      <c r="C67" s="5" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A64" s="10" t="s">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="10" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A65" s="5" t="s">
+    <row r="69" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A69" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="C65" s="5" t="s">
+      <c r="C69" s="5" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" s="8" t="s">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="C66" s="16" t="s">
+      <c r="C70" s="16" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A67" s="17" t="s">
+    <row r="71" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A71" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="C67" s="27" t="s">
+      <c r="C71" s="27" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A68" s="28" t="s">
+    <row r="72" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A72" s="28" t="s">
         <v>196</v>
       </c>
-      <c r="C68" s="5" t="s">
+      <c r="C72" s="5" t="s">
         <v>189</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A69" s="17" t="s">
-        <v>191</v>
-      </c>
-      <c r="C69" s="29" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="144" x14ac:dyDescent="0.3">
-      <c r="A70" s="28" t="s">
-        <v>197</v>
-      </c>
-      <c r="C70" s="5" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A71" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="C71" s="5" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A72" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="C72" s="5" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A73" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="C73" s="29" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+      <c r="A74" s="28" t="s">
+        <v>197</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A75" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A76" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A77" s="17" t="s">
         <v>200</v>
       </c>
-      <c r="C73" s="29" t="s">
+      <c r="C77" s="29" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A74" s="5" t="s">
+    <row r="78" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A78" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="B74" s="5" t="s">
+      <c r="B78" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="C74" s="5" t="s">
+      <c r="C78" s="5" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="B75" s="5" t="s">
+    <row r="79" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B79" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="C75" s="30" t="s">
+      <c r="C79" s="30" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A76" s="5" t="s">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="C76" s="5" t="s">
+      <c r="C80" s="5" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A77" s="5" t="s">
+    <row r="81" spans="1:22" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A81" s="5" t="s">
         <v>364</v>
       </c>
-      <c r="B77" s="5" t="s">
+      <c r="B81" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="C77" s="5" t="s">
+      <c r="C81" s="5" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A78" s="5" t="s">
+    <row r="82" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A82" s="5" t="s">
         <v>365</v>
       </c>
-      <c r="B78" s="5" t="s">
+      <c r="B82" s="5" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B80"/>
-    </row>
-    <row r="81" spans="1:22" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="31"/>
-      <c r="B81" s="32"/>
-      <c r="C81" s="33"/>
-      <c r="D81" s="31"/>
-      <c r="E81" s="34"/>
-      <c r="F81" s="31"/>
-      <c r="G81" s="32"/>
-      <c r="H81" s="31"/>
-      <c r="I81" s="31"/>
-      <c r="J81" s="34"/>
-      <c r="K81" s="31"/>
-      <c r="L81" s="31"/>
-      <c r="M81" s="31"/>
-      <c r="N81" s="31"/>
-      <c r="O81" s="34"/>
-      <c r="P81" s="32"/>
-      <c r="Q81" s="32"/>
-      <c r="R81" s="32"/>
-      <c r="S81" s="32"/>
-      <c r="T81" s="35"/>
-      <c r="U81" s="32"/>
-    </row>
-    <row r="82" spans="1:22" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="36" t="s">
+    <row r="84" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B84"/>
+    </row>
+    <row r="85" spans="1:22" s="36" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="31"/>
+      <c r="B85" s="32"/>
+      <c r="C85" s="33"/>
+      <c r="D85" s="31"/>
+      <c r="E85" s="34"/>
+      <c r="F85" s="31"/>
+      <c r="G85" s="32"/>
+      <c r="H85" s="31"/>
+      <c r="I85" s="31"/>
+      <c r="J85" s="34"/>
+      <c r="K85" s="31"/>
+      <c r="L85" s="31"/>
+      <c r="M85" s="31"/>
+      <c r="N85" s="31"/>
+      <c r="O85" s="34"/>
+      <c r="P85" s="32"/>
+      <c r="Q85" s="32"/>
+      <c r="R85" s="32"/>
+      <c r="S85" s="32"/>
+      <c r="T85" s="35"/>
+      <c r="U85" s="32"/>
+    </row>
+    <row r="86" spans="1:22" s="36" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="36" t="s">
         <v>221</v>
       </c>
-      <c r="B82" s="37"/>
-      <c r="C82" s="52" t="s">
+      <c r="B86" s="37"/>
+      <c r="C86" s="52" t="s">
         <v>306</v>
       </c>
-      <c r="E82" s="34"/>
-      <c r="G82" s="37"/>
-      <c r="J82" s="34"/>
-      <c r="O82" s="34"/>
-      <c r="Q82" s="37"/>
-      <c r="R82" s="37"/>
-      <c r="T82" s="35"/>
-      <c r="V82" s="37"/>
-    </row>
-    <row r="83" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A83" s="43"/>
-      <c r="B83" s="44" t="s">
+      <c r="E86" s="34"/>
+      <c r="G86" s="37"/>
+      <c r="J86" s="34"/>
+      <c r="O86" s="34"/>
+      <c r="Q86" s="37"/>
+      <c r="R86" s="37"/>
+      <c r="T86" s="35"/>
+      <c r="V86" s="37"/>
+    </row>
+    <row r="87" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A87" s="43"/>
+      <c r="B87" s="44" t="s">
         <v>223</v>
       </c>
-      <c r="C83" s="44"/>
-      <c r="D83" s="45"/>
-    </row>
-    <row r="84" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A84" s="46"/>
-      <c r="C84" s="5" t="s">
+      <c r="C87" s="44"/>
+      <c r="D87" s="45"/>
+    </row>
+    <row r="88" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A88" s="46"/>
+      <c r="C88" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="D84" s="47"/>
-    </row>
-    <row r="85" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A85" s="46"/>
-      <c r="B85" s="5" t="s">
+      <c r="D88" s="47"/>
+    </row>
+    <row r="89" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A89" s="46"/>
+      <c r="B89" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="C85" s="5" t="s">
+      <c r="C89" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="D85" s="47"/>
-    </row>
-    <row r="86" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A86" s="46" t="s">
+      <c r="D89" s="47"/>
+    </row>
+    <row r="90" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A90" s="46" t="s">
         <v>219</v>
       </c>
-      <c r="C86" s="5" t="s">
+      <c r="C90" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="D86" s="47"/>
-    </row>
-    <row r="87" spans="1:22" ht="72" x14ac:dyDescent="0.3">
-      <c r="A87" s="46" t="s">
+      <c r="D90" s="47"/>
+    </row>
+    <row r="91" spans="1:22" ht="72" x14ac:dyDescent="0.3">
+      <c r="A91" s="46" t="s">
         <v>232</v>
       </c>
-      <c r="C87" s="5" t="s">
+      <c r="C91" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="D87" s="47"/>
-    </row>
-    <row r="88" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A88" s="46" t="s">
+      <c r="D91" s="47"/>
+    </row>
+    <row r="92" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A92" s="46" t="s">
         <v>226</v>
       </c>
-      <c r="B88" s="5" t="s">
+      <c r="B92" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="C88" s="5" t="s">
+      <c r="C92" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="D88" s="47"/>
-    </row>
-    <row r="89" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A89" s="46" t="s">
+      <c r="D92" s="47"/>
+    </row>
+    <row r="93" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A93" s="46" t="s">
         <v>229</v>
       </c>
-      <c r="C89" s="5" t="s">
+      <c r="C93" s="5" t="s">
         <v>230</v>
-      </c>
-      <c r="D89" s="47"/>
-    </row>
-    <row r="90" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A90" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="B90" s="49" t="s">
-        <v>247</v>
-      </c>
-      <c r="C90" s="49" t="s">
-        <v>231</v>
-      </c>
-      <c r="D90" s="50"/>
-    </row>
-    <row r="91" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A91" s="43"/>
-      <c r="B91" s="44" t="s">
-        <v>235</v>
-      </c>
-      <c r="C91" s="44"/>
-      <c r="D91" s="45"/>
-    </row>
-    <row r="92" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A92" s="46" t="s">
-        <v>165</v>
-      </c>
-      <c r="C92" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="D92" s="47"/>
-    </row>
-    <row r="93" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A93" s="46" t="s">
-        <v>237</v>
-      </c>
-      <c r="B93" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="C93" s="5" t="s">
-        <v>261</v>
       </c>
       <c r="D93" s="47"/>
     </row>
     <row r="94" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A94" s="48" t="s">
-        <v>238</v>
+        <v>67</v>
       </c>
       <c r="B94" s="49" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="C94" s="49" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="D94" s="50"/>
     </row>
     <row r="95" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A95" s="43"/>
       <c r="B95" s="44" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="C95" s="44"/>
       <c r="D95" s="45"/>
     </row>
-    <row r="96" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A96" s="46"/>
+    <row r="96" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A96" s="46" t="s">
+        <v>165</v>
+      </c>
       <c r="C96" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D96" s="47"/>
+    </row>
+    <row r="97" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A97" s="46" t="s">
+        <v>237</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="D97" s="47"/>
+    </row>
+    <row r="98" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A98" s="48" t="s">
+        <v>238</v>
+      </c>
+      <c r="B98" s="49" t="s">
+        <v>241</v>
+      </c>
+      <c r="C98" s="49" t="s">
+        <v>239</v>
+      </c>
+      <c r="D98" s="50"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A99" s="43"/>
+      <c r="B99" s="44" t="s">
+        <v>242</v>
+      </c>
+      <c r="C99" s="44"/>
+      <c r="D99" s="45"/>
+    </row>
+    <row r="100" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A100" s="46"/>
+      <c r="C100" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="D96" s="47"/>
-    </row>
-    <row r="97" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A97" s="46" t="s">
+      <c r="D100" s="47"/>
+    </row>
+    <row r="101" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A101" s="46" t="s">
         <v>244</v>
       </c>
-      <c r="D97" s="47" t="s">
+      <c r="D101" s="47" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A98" s="38"/>
-      <c r="B98" s="5" t="s">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102" s="38"/>
+      <c r="B102" s="5" t="s">
         <v>288</v>
       </c>
-      <c r="D98" s="3" t="s">
+      <c r="D102" s="3" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B99" s="40" t="s">
+    <row r="103" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B103" s="40" t="s">
         <v>282</v>
       </c>
-      <c r="C99" s="5" t="s">
+      <c r="C103" s="5" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A100" s="5" t="s">
+    <row r="104" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A104" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="B100" s="5" t="s">
+      <c r="B104" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="C100" s="5" t="s">
+      <c r="C104" s="5" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A101" s="5" t="s">
+    <row r="105" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A105" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="B101" s="5" t="s">
+      <c r="B105" s="5" t="s">
         <v>486</v>
       </c>
-      <c r="C101" s="5" t="s">
+      <c r="C105" s="5" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A102" s="5" t="s">
+    <row r="106" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A106" s="5" t="s">
         <v>487</v>
       </c>
-      <c r="C102" s="5" t="s">
+      <c r="C106" s="5" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A103" s="5" t="s">
+    <row r="107" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A107" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="C103" s="59" t="s">
+      <c r="C107" s="59" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A104" s="5" t="s">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A108" s="5" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A105" s="5" t="s">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A109" s="5" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A106" s="5" t="s">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A110" s="5" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A107" s="43"/>
-      <c r="B107" s="44" t="s">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A111" s="43"/>
+      <c r="B111" s="44" t="s">
         <v>288</v>
       </c>
-      <c r="C107" s="44"/>
-      <c r="D107" s="45"/>
-    </row>
-    <row r="108" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A108" s="46"/>
-      <c r="C108" s="5" t="s">
+      <c r="C111" s="44"/>
+      <c r="D111" s="45"/>
+    </row>
+    <row r="112" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A112" s="46"/>
+      <c r="C112" s="5" t="s">
         <v>444</v>
       </c>
-      <c r="D108" s="47"/>
-    </row>
-    <row r="109" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A109" s="46" t="s">
+      <c r="D112" s="47"/>
+    </row>
+    <row r="113" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A113" s="46" t="s">
         <v>446</v>
       </c>
-      <c r="C109" s="5" t="s">
+      <c r="C113" s="5" t="s">
         <v>445</v>
-      </c>
-      <c r="D109" s="47"/>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A110" s="46" t="s">
-        <v>165</v>
-      </c>
-      <c r="C110" s="5" t="s">
-        <v>447</v>
-      </c>
-      <c r="D110" s="47"/>
-    </row>
-    <row r="111" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A111" s="46" t="s">
-        <v>448</v>
-      </c>
-      <c r="C111" s="5" t="s">
-        <v>449</v>
-      </c>
-      <c r="D111" s="47"/>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B112" s="46" t="s">
-        <v>457</v>
-      </c>
-      <c r="D112" s="47"/>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A113" s="46" t="s">
-        <v>450</v>
-      </c>
-      <c r="B113" s="5" t="s">
-        <v>452</v>
-      </c>
-      <c r="C113" s="5" t="s">
-        <v>451</v>
       </c>
       <c r="D113" s="47"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="46" t="s">
+        <v>165</v>
+      </c>
+      <c r="C114" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="D114" s="47"/>
+    </row>
+    <row r="115" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A115" s="46" t="s">
+        <v>448</v>
+      </c>
+      <c r="C115" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="D115" s="47"/>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B116" s="46" t="s">
+        <v>457</v>
+      </c>
+      <c r="D116" s="47"/>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A117" s="46" t="s">
+        <v>450</v>
+      </c>
+      <c r="B117" s="5" t="s">
+        <v>452</v>
+      </c>
+      <c r="C117" s="5" t="s">
+        <v>451</v>
+      </c>
+      <c r="D117" s="47"/>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A118" s="46" t="s">
         <v>453</v>
       </c>
-      <c r="B114" s="5" t="s">
+      <c r="B118" s="5" t="s">
         <v>454</v>
       </c>
-      <c r="C114" s="5" t="s">
+      <c r="C118" s="5" t="s">
         <v>451</v>
       </c>
-      <c r="D114" s="47"/>
-    </row>
-    <row r="115" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A115" s="48" t="s">
+      <c r="D118" s="47"/>
+    </row>
+    <row r="119" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A119" s="48" t="s">
         <v>455</v>
       </c>
-      <c r="B115" s="49"/>
-      <c r="C115" s="49" t="s">
+      <c r="B119" s="49"/>
+      <c r="C119" s="49" t="s">
         <v>456</v>
       </c>
-      <c r="D115" s="50"/>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A116" s="46"/>
-      <c r="B116" s="46" t="s">
+      <c r="D119" s="50"/>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A120" s="46"/>
+      <c r="B120" s="46" t="s">
         <v>458</v>
       </c>
-      <c r="D116" s="47"/>
-    </row>
-    <row r="117" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A117" s="46" t="s">
+      <c r="D120" s="47"/>
+    </row>
+    <row r="121" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A121" s="46" t="s">
         <v>448</v>
       </c>
-      <c r="C117" s="5" t="s">
+      <c r="C121" s="5" t="s">
         <v>449</v>
       </c>
-      <c r="D117" s="47"/>
-    </row>
-    <row r="118" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A118" s="46" t="s">
+      <c r="D121" s="47"/>
+    </row>
+    <row r="122" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A122" s="46" t="s">
         <v>459</v>
       </c>
-      <c r="B118" s="5" t="s">
+      <c r="B122" s="5" t="s">
         <v>461</v>
       </c>
-      <c r="C118" s="5" t="s">
+      <c r="C122" s="5" t="s">
         <v>460</v>
       </c>
-      <c r="D118" s="47"/>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A119" s="43"/>
-      <c r="B119" s="44" t="s">
+      <c r="D122" s="47"/>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A123" s="43"/>
+      <c r="B123" s="44" t="s">
         <v>287</v>
       </c>
-      <c r="C119" s="44"/>
-      <c r="D119" s="45"/>
-    </row>
-    <row r="120" spans="1:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="A120" s="46"/>
-      <c r="B120" s="40" t="s">
+      <c r="C123" s="44"/>
+      <c r="D123" s="45"/>
+    </row>
+    <row r="124" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A124" s="46"/>
+      <c r="B124" s="40" t="s">
         <v>283</v>
       </c>
-      <c r="D120" s="47"/>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A121" s="46" t="s">
+      <c r="D124" s="47"/>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A125" s="46" t="s">
         <v>284</v>
       </c>
-      <c r="D121" s="47"/>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A122" s="46" t="s">
+      <c r="D125" s="47"/>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A126" s="46" t="s">
         <v>249</v>
       </c>
-      <c r="D122" s="47"/>
-    </row>
-    <row r="123" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A123" s="48" t="s">
+      <c r="D126" s="47"/>
+    </row>
+    <row r="127" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A127" s="48" t="s">
         <v>285</v>
       </c>
-      <c r="B123" s="49"/>
-      <c r="C123" s="49" t="s">
+      <c r="B127" s="49"/>
+      <c r="C127" s="49" t="s">
         <v>286</v>
       </c>
-      <c r="D123" s="50"/>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A124" s="43"/>
-      <c r="B124" s="44" t="s">
+      <c r="D127" s="50"/>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A128" s="43"/>
+      <c r="B128" s="44" t="s">
         <v>251</v>
       </c>
-      <c r="C124" s="44"/>
-      <c r="D124" s="45"/>
-    </row>
-    <row r="125" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A125" s="46"/>
-      <c r="C125" s="5" t="s">
+      <c r="C128" s="44"/>
+      <c r="D128" s="45"/>
+    </row>
+    <row r="129" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A129" s="46"/>
+      <c r="C129" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="D125" s="47"/>
-    </row>
-    <row r="126" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A126" s="46"/>
-      <c r="C126" s="5" t="s">
+      <c r="D129" s="47"/>
+    </row>
+    <row r="130" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A130" s="46"/>
+      <c r="C130" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="D126" s="47"/>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A127" s="46" t="s">
+      <c r="D130" s="47"/>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A131" s="46" t="s">
         <v>254</v>
       </c>
-      <c r="C127" s="5" t="s">
+      <c r="C131" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="D127" s="47"/>
-    </row>
-    <row r="128" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A128" s="46" t="s">
+      <c r="D131" s="47"/>
+    </row>
+    <row r="132" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A132" s="46" t="s">
         <v>255</v>
       </c>
-      <c r="C128" s="5" t="s">
+      <c r="C132" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="D128" s="47"/>
-    </row>
-    <row r="129" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A129" s="46" t="s">
+      <c r="D132" s="47"/>
+    </row>
+    <row r="133" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A133" s="46" t="s">
         <v>256</v>
       </c>
-      <c r="C129" s="5" t="s">
+      <c r="C133" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="D129" s="47"/>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A130" s="48" t="s">
+      <c r="D133" s="47"/>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A134" s="48" t="s">
         <v>260</v>
       </c>
-      <c r="B130" s="49"/>
-      <c r="C130" s="49"/>
-      <c r="D130" s="50"/>
-    </row>
-    <row r="132" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A133" s="41" t="s">
+      <c r="B134" s="49"/>
+      <c r="C134" s="49"/>
+      <c r="D134" s="50"/>
+    </row>
+    <row r="136" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A137" s="41" t="s">
         <v>265</v>
       </c>
-      <c r="B133" s="19"/>
-      <c r="C133" s="51" t="s">
+      <c r="B137" s="19"/>
+      <c r="C137" s="51" t="s">
         <v>305</v>
       </c>
-      <c r="D133" s="20"/>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A134" s="21" t="s">
+      <c r="D137" s="20"/>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A138" s="21" t="s">
         <v>279</v>
       </c>
-      <c r="C134" s="5" t="s">
+      <c r="C138" s="5" t="s">
         <v>280</v>
       </c>
-      <c r="D134" s="22"/>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A135" s="21" t="s">
+      <c r="D138" s="22"/>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A139" s="21" t="s">
         <v>266</v>
       </c>
-      <c r="C135" s="5" t="s">
+      <c r="C139" s="5" t="s">
         <v>278</v>
-      </c>
-      <c r="D135" s="22"/>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A136" s="21" t="s">
-        <v>289</v>
-      </c>
-      <c r="C136" s="5" t="s">
-        <v>290</v>
-      </c>
-      <c r="D136" s="22"/>
-    </row>
-    <row r="137" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A137" s="21" t="s">
-        <v>292</v>
-      </c>
-      <c r="C137" s="5" t="s">
-        <v>297</v>
-      </c>
-      <c r="D137" s="22"/>
-    </row>
-    <row r="138" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A138" s="21" t="s">
-        <v>296</v>
-      </c>
-      <c r="C138" s="5" t="s">
-        <v>286</v>
-      </c>
-      <c r="D138" s="22"/>
-    </row>
-    <row r="139" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A139" s="21" t="s">
-        <v>293</v>
-      </c>
-      <c r="C139" s="5" t="s">
-        <v>298</v>
       </c>
       <c r="D139" s="22"/>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" s="21" t="s">
-        <v>267</v>
+        <v>289</v>
       </c>
       <c r="C140" s="5" t="s">
-        <v>320</v>
+        <v>290</v>
       </c>
       <c r="D140" s="22"/>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A141" s="21" t="s">
-        <v>321</v>
+        <v>292</v>
       </c>
       <c r="C141" s="5" t="s">
-        <v>319</v>
+        <v>297</v>
       </c>
       <c r="D141" s="22"/>
     </row>
     <row r="142" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A142" s="21" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="C142" s="5" t="s">
-        <v>299</v>
+        <v>286</v>
       </c>
       <c r="D142" s="22"/>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A143" s="21" t="s">
-        <v>249</v>
+        <v>293</v>
       </c>
       <c r="C143" s="5" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D143" s="22"/>
     </row>
-    <row r="144" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A144" s="42" t="s">
-        <v>273</v>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A144" s="21" t="s">
+        <v>267</v>
+      </c>
+      <c r="C144" s="5" t="s">
+        <v>320</v>
       </c>
       <c r="D144" s="22"/>
     </row>
-    <row r="145" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A145" s="21" t="s">
-        <v>291</v>
+        <v>321</v>
+      </c>
+      <c r="C145" s="5" t="s">
+        <v>319</v>
       </c>
       <c r="D145" s="22"/>
     </row>
     <row r="146" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A146" s="21" t="s">
+        <v>294</v>
+      </c>
+      <c r="C146" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="D146" s="22"/>
+    </row>
+    <row r="147" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A147" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="C147" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="D147" s="22"/>
+    </row>
+    <row r="148" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A148" s="42" t="s">
+        <v>273</v>
+      </c>
+      <c r="D148" s="22"/>
+    </row>
+    <row r="149" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A149" s="21" t="s">
+        <v>291</v>
+      </c>
+      <c r="D149" s="22"/>
+    </row>
+    <row r="150" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A150" s="21" t="s">
         <v>165</v>
       </c>
-      <c r="C146" s="5" t="s">
+      <c r="C150" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="D146" s="22"/>
-    </row>
-    <row r="147" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A147" s="21" t="s">
+      <c r="D150" s="22"/>
+    </row>
+    <row r="151" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A151" s="21" t="s">
         <v>271</v>
       </c>
-      <c r="C147" s="5" t="s">
+      <c r="C151" s="5" t="s">
         <v>303</v>
       </c>
-      <c r="D147" s="22"/>
-    </row>
-    <row r="148" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A148" s="21" t="s">
+      <c r="D151" s="22"/>
+    </row>
+    <row r="152" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A152" s="21" t="s">
         <v>295</v>
       </c>
-      <c r="C148" s="5" t="s">
+      <c r="C152" s="5" t="s">
         <v>302</v>
       </c>
-      <c r="D148" s="22"/>
-    </row>
-    <row r="149" spans="1:22" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A149" s="23" t="s">
+      <c r="D152" s="22"/>
+    </row>
+    <row r="153" spans="1:22" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A153" s="23" t="s">
         <v>272</v>
       </c>
-      <c r="B149" s="24"/>
-      <c r="C149" s="24" t="s">
+      <c r="B153" s="24"/>
+      <c r="C153" s="24" t="s">
         <v>301</v>
       </c>
-      <c r="D149" s="25"/>
-    </row>
-    <row r="151" spans="1:22" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A151" s="31"/>
-      <c r="B151" s="32"/>
-      <c r="C151" s="33"/>
-      <c r="D151" s="31"/>
-      <c r="E151" s="34"/>
-      <c r="F151" s="31"/>
-      <c r="G151" s="32"/>
-      <c r="H151" s="31"/>
-      <c r="I151" s="31"/>
-      <c r="J151" s="34"/>
-      <c r="K151" s="31"/>
-      <c r="L151" s="31"/>
-      <c r="M151" s="31"/>
-      <c r="N151" s="31"/>
-      <c r="O151" s="34"/>
-      <c r="P151" s="32"/>
-      <c r="Q151" s="32"/>
-      <c r="R151" s="32"/>
-      <c r="S151" s="32"/>
-      <c r="T151" s="35"/>
-      <c r="U151" s="32"/>
-    </row>
-    <row r="152" spans="1:22" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A152" s="36" t="s">
+      <c r="D153" s="25"/>
+    </row>
+    <row r="155" spans="1:22" s="36" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A155" s="31"/>
+      <c r="B155" s="32"/>
+      <c r="C155" s="33"/>
+      <c r="D155" s="31"/>
+      <c r="E155" s="34"/>
+      <c r="F155" s="31"/>
+      <c r="G155" s="32"/>
+      <c r="H155" s="31"/>
+      <c r="I155" s="31"/>
+      <c r="J155" s="34"/>
+      <c r="K155" s="31"/>
+      <c r="L155" s="31"/>
+      <c r="M155" s="31"/>
+      <c r="N155" s="31"/>
+      <c r="O155" s="34"/>
+      <c r="P155" s="32"/>
+      <c r="Q155" s="32"/>
+      <c r="R155" s="32"/>
+      <c r="S155" s="32"/>
+      <c r="T155" s="35"/>
+      <c r="U155" s="32"/>
+    </row>
+    <row r="156" spans="1:22" s="36" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A156" s="36" t="s">
         <v>304</v>
       </c>
-      <c r="B152" s="37"/>
-      <c r="C152" s="39" t="s">
+      <c r="B156" s="37"/>
+      <c r="C156" s="39" t="s">
         <v>222</v>
       </c>
-      <c r="E152" s="34"/>
-      <c r="G152" s="37"/>
-      <c r="J152" s="34"/>
-      <c r="O152" s="34"/>
-      <c r="Q152" s="37"/>
-      <c r="R152" s="37"/>
-      <c r="T152" s="35"/>
-      <c r="V152" s="37"/>
-    </row>
-    <row r="153" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A153" s="38" t="s">
+      <c r="E156" s="34"/>
+      <c r="G156" s="37"/>
+      <c r="J156" s="34"/>
+      <c r="O156" s="34"/>
+      <c r="Q156" s="37"/>
+      <c r="R156" s="37"/>
+      <c r="T156" s="35"/>
+      <c r="V156" s="37"/>
+    </row>
+    <row r="157" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A157" s="38" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="154" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A154" s="5" t="s">
+    <row r="158" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A158" s="5" t="s">
         <v>307</v>
       </c>
-      <c r="C154" s="5" t="s">
+      <c r="C158" s="5" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="155" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A155" s="5" t="s">
+    <row r="159" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A159" s="5" t="s">
         <v>462</v>
       </c>
-      <c r="C155" s="5" t="s">
+      <c r="C159" s="5" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="156" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A156" s="5" t="s">
+    <row r="160" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A160" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="C156" s="5" t="s">
+      <c r="C160" s="5" t="s">
         <v>322</v>
       </c>
-      <c r="D156" s="3" t="s">
+      <c r="D160" s="3" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="157" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A157" s="5" t="s">
+    <row r="161" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A161" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C157" s="5" t="s">
+      <c r="C161" s="5" t="s">
         <v>311</v>
       </c>
-      <c r="D157" s="3" t="s">
+      <c r="D161" s="3" t="s">
         <v>312</v>
-      </c>
-    </row>
-    <row r="158" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A158" s="5" t="s">
-        <v>329</v>
-      </c>
-      <c r="B158" s="5" t="s">
-        <v>331</v>
-      </c>
-      <c r="C158" s="5" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="159" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A159" s="5" t="s">
-        <v>465</v>
-      </c>
-      <c r="B159" s="5" t="s">
-        <v>464</v>
-      </c>
-      <c r="C159" s="5" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="160" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A160" s="5" t="s">
-        <v>313</v>
-      </c>
-      <c r="C160" s="5" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A161" s="5" t="s">
-        <v>323</v>
-      </c>
-      <c r="B161" s="40" t="s">
-        <v>326</v>
-      </c>
-      <c r="C161" s="5" t="s">
-        <v>325</v>
-      </c>
-      <c r="D161" s="3" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="162" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A162" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="B162" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="C162" s="5" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A163" s="5" t="s">
+        <v>465</v>
+      </c>
+      <c r="B163" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="C163" s="5" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A164" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="C164" s="5" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A165" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="B165" s="40" t="s">
+        <v>326</v>
+      </c>
+      <c r="C165" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="D165" s="3" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A166" s="5" t="s">
         <v>327</v>
       </c>
-      <c r="C162" s="5" t="s">
+      <c r="C166" s="5" t="s">
         <v>332</v>
       </c>
-      <c r="D162" s="3" t="s">
+      <c r="D166" s="3" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A163" s="38" t="s">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A167" s="38" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="164" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A164" s="5" t="s">
+    <row r="168" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A168" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B164" s="5" t="s">
+      <c r="B168" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C164" s="5" t="s">
+      <c r="C168" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="D164" s="9" t="s">
+      <c r="D168" s="9" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="165" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A165" s="40" t="s">
+    <row r="169" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A169" s="40" t="s">
         <v>335</v>
       </c>
-      <c r="B165" s="13" t="s">
+      <c r="B169" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="C165" s="5" t="s">
+      <c r="C169" s="5" t="s">
         <v>337</v>
       </c>
-      <c r="D165" s="5"/>
-    </row>
-    <row r="166" spans="1:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="B166" s="40" t="s">
+      <c r="D169" s="5"/>
+    </row>
+    <row r="170" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="B170" s="40" t="s">
         <v>339</v>
       </c>
-      <c r="C166" s="5" t="s">
+      <c r="C170" s="5" t="s">
         <v>336</v>
       </c>
-      <c r="D166" s="3" t="s">
+      <c r="D170" s="3" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="167" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C167" s="5" t="s">
+    <row r="171" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C171" s="5" t="s">
         <v>338</v>
       </c>
-      <c r="D167" s="3" t="s">
+      <c r="D171" s="3" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A168" s="38" t="s">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A172" s="38" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A169" s="5" t="s">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A173" s="5" t="s">
         <v>342</v>
       </c>
-      <c r="B169" s="5" t="s">
+      <c r="B173" s="5" t="s">
         <v>348</v>
       </c>
-      <c r="C169" s="5" t="s">
+      <c r="C173" s="5" t="s">
         <v>466</v>
       </c>
-      <c r="D169" s="3" t="s">
+      <c r="D173" s="3" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A170" s="5" t="s">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A174" s="5" t="s">
         <v>343</v>
       </c>
-      <c r="B170" s="5" t="s">
+      <c r="B174" s="5" t="s">
         <v>348</v>
       </c>
-      <c r="C170" s="5" t="s">
+      <c r="C174" s="5" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="171" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A171" s="5" t="s">
+    <row r="175" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A175" s="5" t="s">
         <v>352</v>
       </c>
-      <c r="B171" s="5" t="s">
+      <c r="B175" s="5" t="s">
         <v>348</v>
       </c>
-      <c r="C171" s="5" t="s">
+      <c r="C175" s="5" t="s">
         <v>467</v>
       </c>
-      <c r="D171" s="3" t="s">
+      <c r="D175" s="3" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="172" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A172" s="5" t="s">
+    <row r="176" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A176" s="5" t="s">
         <v>344</v>
       </c>
-      <c r="B172" s="5" t="s">
+      <c r="B176" s="5" t="s">
         <v>370</v>
       </c>
-      <c r="C172" s="5" t="s">
+      <c r="C176" s="5" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="173" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A173" s="28" t="s">
+    <row r="177" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A177" s="28" t="s">
         <v>346</v>
       </c>
-      <c r="B173" s="5" t="s">
+      <c r="B177" s="5" t="s">
         <v>522</v>
       </c>
-      <c r="C173" s="5" t="s">
+      <c r="C177" s="5" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="174" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A174" s="28" t="s">
+    <row r="178" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A178" s="28" t="s">
         <v>523</v>
       </c>
-      <c r="B174" s="5" t="s">
+      <c r="B178" s="5" t="s">
         <v>524</v>
       </c>
-      <c r="C174" s="5" t="s">
+      <c r="C178" s="5" t="s">
         <v>525</v>
       </c>
-      <c r="D174" s="63" t="s">
+      <c r="D178" s="63" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="175" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A175" s="5" t="s">
+    <row r="179" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A179" s="5" t="s">
         <v>345</v>
       </c>
-      <c r="B175" s="5" t="s">
+      <c r="B179" s="5" t="s">
         <v>519</v>
       </c>
-      <c r="C175" s="5" t="s">
+      <c r="C179" s="5" t="s">
         <v>477</v>
       </c>
-      <c r="D175" s="62" t="s">
+      <c r="D179" s="62" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="176" spans="1:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="A176" s="5" t="s">
+    <row r="180" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A180" s="5" t="s">
         <v>472</v>
       </c>
-      <c r="C176" s="5" t="s">
+      <c r="C180" s="5" t="s">
         <v>469</v>
       </c>
-      <c r="D176" s="53"/>
-    </row>
-    <row r="177" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A177" s="5" t="s">
+      <c r="D180" s="53"/>
+    </row>
+    <row r="181" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A181" s="5" t="s">
         <v>473</v>
       </c>
-      <c r="C177" s="5" t="s">
+      <c r="C181" s="5" t="s">
         <v>470</v>
       </c>
-      <c r="D177" s="53"/>
-    </row>
-    <row r="178" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A178" s="5" t="s">
+      <c r="D181" s="53"/>
+    </row>
+    <row r="182" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A182" s="5" t="s">
         <v>474</v>
       </c>
-      <c r="C178" s="5" t="s">
+      <c r="C182" s="5" t="s">
         <v>471</v>
       </c>
-      <c r="D178" s="53"/>
-    </row>
-    <row r="179" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A179" s="5" t="s">
+      <c r="D182" s="53"/>
+    </row>
+    <row r="183" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A183" s="5" t="s">
         <v>531</v>
       </c>
-      <c r="B179" s="5" t="s">
+      <c r="B183" s="5" t="s">
         <v>530</v>
       </c>
-      <c r="C179" s="5" t="s">
+      <c r="C183" s="5" t="s">
         <v>529</v>
       </c>
-      <c r="D179" s="53"/>
-    </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A180" s="38" t="s">
+      <c r="D183" s="53"/>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A184" s="38" t="s">
         <v>354</v>
       </c>
-      <c r="D180" s="3" t="s">
+      <c r="D184" s="3" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C181" s="5" t="s">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C185" s="5" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="182" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A182" s="5" t="s">
+    <row r="186" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A186" s="5" t="s">
         <v>357</v>
       </c>
-      <c r="C182" s="5" t="s">
+      <c r="C186" s="5" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A183" s="5" t="s">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A187" s="5" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="184" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A184" s="5" t="s">
+    <row r="188" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A188" s="5" t="s">
         <v>358</v>
       </c>
-      <c r="C184" s="5" t="s">
+      <c r="C188" s="5" t="s">
         <v>369</v>
       </c>
-      <c r="D184" s="53" t="s">
+      <c r="D188" s="53" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A185" s="5" t="s">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A189" s="5" t="s">
         <v>359</v>
       </c>
-      <c r="C185" s="5" t="s">
+      <c r="C189" s="5" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C186" s="5" t="s">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C190" s="5" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A187" s="5" t="s">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A191" s="5" t="s">
         <v>362</v>
       </c>
-      <c r="C187" s="5" t="s">
+      <c r="C191" s="5" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="188" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C188" s="5" t="s">
+    <row r="192" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C192" s="5" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="189" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A189" s="5" t="s">
+    <row r="193" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A193" s="5" t="s">
         <v>521</v>
       </c>
-      <c r="B189" s="5" t="s">
+      <c r="B193" s="5" t="s">
         <v>407</v>
       </c>
-      <c r="C189" s="5" t="s">
+      <c r="C193" s="5" t="s">
         <v>476</v>
       </c>
-      <c r="D189" s="60" t="s">
+      <c r="D193" s="60" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A190" s="38" t="s">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A194" s="38" t="s">
         <v>372</v>
       </c>
-      <c r="D190" s="3" t="s">
+      <c r="D194" s="3" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="191" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A191" s="5" t="s">
+    <row r="195" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A195" s="5" t="s">
         <v>374</v>
       </c>
-      <c r="B191" s="54" t="s">
+      <c r="B195" s="54" t="s">
         <v>375</v>
       </c>
-      <c r="C191" s="5" t="s">
+      <c r="C195" s="5" t="s">
         <v>518</v>
       </c>
-      <c r="F191" s="5" t="s">
+      <c r="F195" s="5" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A192" s="38" t="s">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A196" s="38" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A193" s="55" t="s">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A197" s="55" t="s">
         <v>378</v>
       </c>
-      <c r="B193" s="44" t="s">
+      <c r="B197" s="44" t="s">
         <v>379</v>
       </c>
-      <c r="C193" s="44" t="s">
+      <c r="C197" s="44" t="s">
         <v>384</v>
       </c>
-      <c r="D193" s="45" t="s">
+      <c r="D197" s="45" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A194" s="46" t="s">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A198" s="46" t="s">
         <v>380</v>
       </c>
-      <c r="D194" s="47"/>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A195" s="48" t="s">
+      <c r="D198" s="47"/>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A199" s="48" t="s">
         <v>381</v>
       </c>
-      <c r="B195" s="49"/>
-      <c r="C195" s="49" t="s">
+      <c r="B199" s="49"/>
+      <c r="C199" s="49" t="s">
         <v>382</v>
       </c>
-      <c r="D195" s="50"/>
-    </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A196" s="55" t="s">
+      <c r="D199" s="50"/>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A200" s="55" t="s">
         <v>378</v>
       </c>
-      <c r="B196" s="44" t="s">
+      <c r="B200" s="44" t="s">
         <v>379</v>
       </c>
-      <c r="C196" s="44" t="s">
+      <c r="C200" s="44" t="s">
         <v>385</v>
       </c>
-      <c r="D196" s="45" t="s">
+      <c r="D200" s="45" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A197" s="46" t="s">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A201" s="46" t="s">
         <v>380</v>
       </c>
-      <c r="D197" s="47"/>
-    </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A198" s="48" t="s">
+      <c r="D201" s="47"/>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A202" s="48" t="s">
         <v>386</v>
       </c>
-      <c r="B198" s="49"/>
-      <c r="C198" s="49" t="s">
+      <c r="B202" s="49"/>
+      <c r="C202" s="49" t="s">
         <v>382</v>
       </c>
-      <c r="D198" s="50"/>
-    </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A199" s="38" t="s">
+      <c r="D202" s="50"/>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A203" s="38" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="200" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A200" s="5" t="s">
+    <row r="204" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A204" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="B200" s="54" t="s">
+      <c r="B204" s="54" t="s">
         <v>392</v>
       </c>
-      <c r="C200" s="5" t="s">
+      <c r="C204" s="5" t="s">
         <v>390</v>
       </c>
-      <c r="D200" s="3" t="s">
+      <c r="D204" s="3" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="201" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A201" s="5" t="s">
+    <row r="205" spans="1:6" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A205" s="5" t="s">
         <v>510</v>
       </c>
-      <c r="B201" s="54" t="s">
+      <c r="B205" s="54" t="s">
         <v>398</v>
       </c>
-      <c r="C201" s="5" t="s">
+      <c r="C205" s="5" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A202" s="5" t="s">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A206" s="5" t="s">
         <v>393</v>
       </c>
-      <c r="C202" s="5" t="s">
+      <c r="C206" s="5" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="203" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A203" s="5" t="s">
+    <row r="207" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A207" s="5" t="s">
         <v>395</v>
       </c>
-      <c r="B203" s="54" t="s">
+      <c r="B207" s="54" t="s">
         <v>396</v>
       </c>
-      <c r="C203" s="5" t="s">
+      <c r="C207" s="5" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A204" s="38" t="s">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A208" s="38" t="s">
         <v>497</v>
       </c>
-      <c r="B204" s="54"/>
-    </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A205" s="5" t="s">
+      <c r="B208" s="54"/>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A209" s="5" t="s">
         <v>498</v>
-      </c>
-      <c r="B205" s="54"/>
-      <c r="C205" s="5" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A206" s="5" t="s">
-        <v>499</v>
-      </c>
-      <c r="B206" s="54"/>
-      <c r="C206" s="5" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A207" s="5" t="s">
-        <v>506</v>
-      </c>
-      <c r="B207" s="54"/>
-      <c r="C207" s="5" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A208" s="5" t="s">
-        <v>500</v>
-      </c>
-      <c r="B208" s="54"/>
-      <c r="C208" s="5" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="209" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A209" s="5" t="s">
-        <v>501</v>
       </c>
       <c r="B209" s="54"/>
       <c r="C209" s="5" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="210" spans="1:22" x14ac:dyDescent="0.3">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" s="5" t="s">
-        <v>508</v>
+        <v>499</v>
       </c>
       <c r="B210" s="54"/>
       <c r="C210" s="5" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A211" s="5" t="s">
+        <v>506</v>
+      </c>
+      <c r="B211" s="54"/>
+      <c r="C211" s="5" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A212" s="5" t="s">
+        <v>500</v>
+      </c>
+      <c r="B212" s="54"/>
+      <c r="C212" s="5" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A213" s="5" t="s">
+        <v>501</v>
+      </c>
+      <c r="B213" s="54"/>
+      <c r="C213" s="5" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A214" s="5" t="s">
+        <v>508</v>
+      </c>
+      <c r="B214" s="54"/>
+      <c r="C214" s="5" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="211" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="B211" s="54"/>
-    </row>
-    <row r="212" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A212" s="38" t="s">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B215" s="54"/>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A216" s="38" t="s">
         <v>399</v>
       </c>
-      <c r="D212" s="3" t="s">
+      <c r="D216" s="3" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="213" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A213" s="5" t="s">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A217" s="5" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="214" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A214" s="5" t="s">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A218" s="5" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="215" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A215" s="5" t="s">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A219" s="5" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="216" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A216" s="5" t="s">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A220" s="5" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="217" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A217" s="5" t="s">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A221" s="5" t="s">
         <v>514</v>
       </c>
-      <c r="C217" s="5" t="s">
+      <c r="C221" s="5" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="218" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A218" s="5" t="s">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A222" s="5" t="s">
         <v>515</v>
       </c>
-      <c r="C218" s="5" t="s">
+      <c r="C222" s="5" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="221" spans="1:22" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A221" s="31"/>
-      <c r="B221" s="32"/>
-      <c r="C221" s="33"/>
-      <c r="D221" s="31"/>
-      <c r="E221" s="34"/>
-      <c r="F221" s="31"/>
-      <c r="G221" s="32"/>
-      <c r="H221" s="31"/>
-      <c r="I221" s="31"/>
-      <c r="J221" s="34"/>
-      <c r="K221" s="31"/>
-      <c r="L221" s="31"/>
-      <c r="M221" s="31"/>
-      <c r="N221" s="31"/>
-      <c r="O221" s="34"/>
-      <c r="P221" s="32"/>
-      <c r="Q221" s="32"/>
-      <c r="R221" s="32"/>
-      <c r="S221" s="32"/>
-      <c r="T221" s="35"/>
-      <c r="U221" s="32"/>
-    </row>
-    <row r="222" spans="1:22" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A222" s="36" t="s">
+    <row r="225" spans="1:22" s="36" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A225" s="31"/>
+      <c r="B225" s="32"/>
+      <c r="C225" s="33"/>
+      <c r="D225" s="31"/>
+      <c r="E225" s="34"/>
+      <c r="F225" s="31"/>
+      <c r="G225" s="32"/>
+      <c r="H225" s="31"/>
+      <c r="I225" s="31"/>
+      <c r="J225" s="34"/>
+      <c r="K225" s="31"/>
+      <c r="L225" s="31"/>
+      <c r="M225" s="31"/>
+      <c r="N225" s="31"/>
+      <c r="O225" s="34"/>
+      <c r="P225" s="32"/>
+      <c r="Q225" s="32"/>
+      <c r="R225" s="32"/>
+      <c r="S225" s="32"/>
+      <c r="T225" s="35"/>
+      <c r="U225" s="32"/>
+    </row>
+    <row r="226" spans="1:22" s="36" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A226" s="36" t="s">
         <v>478</v>
       </c>
-      <c r="B222" s="37"/>
-      <c r="C222" s="56"/>
-      <c r="E222" s="34"/>
-      <c r="G222" s="37"/>
-      <c r="J222" s="34"/>
-      <c r="O222" s="34"/>
-      <c r="Q222" s="37"/>
-      <c r="R222" s="37"/>
-      <c r="T222" s="35"/>
-      <c r="V222" s="37"/>
-    </row>
-    <row r="223" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A223" s="38" t="s">
+      <c r="B226" s="37"/>
+      <c r="C226" s="56"/>
+      <c r="E226" s="34"/>
+      <c r="G226" s="37"/>
+      <c r="J226" s="34"/>
+      <c r="O226" s="34"/>
+      <c r="Q226" s="37"/>
+      <c r="R226" s="37"/>
+      <c r="T226" s="35"/>
+      <c r="V226" s="37"/>
+    </row>
+    <row r="227" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A227" s="38" t="s">
         <v>124</v>
       </c>
-      <c r="D223" s="3" t="s">
+      <c r="D227" s="3" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="224" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A224" s="5" t="s">
+    <row r="228" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A228" s="5" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="225" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A225" s="38" t="s">
+    <row r="229" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A229" s="38" t="s">
         <v>481</v>
       </c>
-      <c r="C225" s="5" t="s">
+      <c r="C229" s="5" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="226" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="B226" s="5" t="s">
+    <row r="230" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="B230" s="5" t="s">
         <v>457</v>
       </c>
-      <c r="C226" s="5" t="s">
+      <c r="C230" s="5" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="227" spans="1:22" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="B227" s="5" t="s">
+    <row r="231" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="B231" s="5" t="s">
         <v>458</v>
       </c>
-      <c r="C227" s="5" t="s">
+      <c r="C231" s="5" t="s">
         <v>484</v>
       </c>
-      <c r="D227" s="3" t="s">
+      <c r="D231" s="3" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="238" spans="1:22" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A238" s="31"/>
-      <c r="B238" s="32"/>
-      <c r="C238" s="33"/>
-      <c r="D238" s="31"/>
-      <c r="E238" s="34"/>
-      <c r="F238" s="31"/>
-      <c r="G238" s="32"/>
-      <c r="H238" s="31"/>
-      <c r="I238" s="31"/>
-      <c r="J238" s="34"/>
-      <c r="K238" s="31"/>
-      <c r="L238" s="31"/>
-      <c r="M238" s="31"/>
-      <c r="N238" s="31"/>
-      <c r="O238" s="34"/>
-      <c r="P238" s="32"/>
-      <c r="Q238" s="32"/>
-      <c r="R238" s="32"/>
-      <c r="S238" s="32"/>
-      <c r="T238" s="35"/>
-      <c r="U238" s="32"/>
-    </row>
-    <row r="239" spans="1:22" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A239" s="36" t="s">
+    <row r="242" spans="1:22" s="36" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A242" s="31"/>
+      <c r="B242" s="32"/>
+      <c r="C242" s="33"/>
+      <c r="D242" s="31"/>
+      <c r="E242" s="34"/>
+      <c r="F242" s="31"/>
+      <c r="G242" s="32"/>
+      <c r="H242" s="31"/>
+      <c r="I242" s="31"/>
+      <c r="J242" s="34"/>
+      <c r="K242" s="31"/>
+      <c r="L242" s="31"/>
+      <c r="M242" s="31"/>
+      <c r="N242" s="31"/>
+      <c r="O242" s="34"/>
+      <c r="P242" s="32"/>
+      <c r="Q242" s="32"/>
+      <c r="R242" s="32"/>
+      <c r="S242" s="32"/>
+      <c r="T242" s="35"/>
+      <c r="U242" s="32"/>
+    </row>
+    <row r="243" spans="1:22" s="36" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A243" s="36" t="s">
         <v>403</v>
       </c>
-      <c r="B239" s="37"/>
-      <c r="C239" s="56" t="s">
+      <c r="B243" s="37"/>
+      <c r="C243" s="56" t="s">
         <v>404</v>
       </c>
-      <c r="E239" s="34"/>
-      <c r="G239" s="37"/>
-      <c r="J239" s="34"/>
-      <c r="O239" s="34"/>
-      <c r="Q239" s="37"/>
-      <c r="R239" s="37"/>
-      <c r="T239" s="35"/>
-      <c r="V239" s="37"/>
-    </row>
-    <row r="240" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A240" s="38" t="s">
+      <c r="E243" s="34"/>
+      <c r="G243" s="37"/>
+      <c r="J243" s="34"/>
+      <c r="O243" s="34"/>
+      <c r="Q243" s="37"/>
+      <c r="R243" s="37"/>
+      <c r="T243" s="35"/>
+      <c r="V243" s="37"/>
+    </row>
+    <row r="244" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A244" s="38" t="s">
         <v>406</v>
       </c>
-      <c r="C240" s="5" t="s">
+      <c r="C244" s="5" t="s">
         <v>409</v>
       </c>
-      <c r="D240" s="3" t="s">
+      <c r="D244" s="3" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="241" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A241" s="57" t="s">
+    <row r="245" spans="1:22" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A245" s="57" t="s">
         <v>414</v>
       </c>
-      <c r="B241" s="5" t="s">
+      <c r="B245" s="5" t="s">
         <v>408</v>
       </c>
-      <c r="C241" s="57" t="s">
+      <c r="C245" s="57" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="242" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A242" s="5" t="s">
+    <row r="246" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A246" s="5" t="s">
         <v>411</v>
       </c>
-      <c r="C242" s="57" t="s">
+      <c r="C246" s="57" t="s">
         <v>413</v>
       </c>
-      <c r="D242" s="3" t="s">
+      <c r="D246" s="3" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A243" s="38" t="s">
+    <row r="247" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A247" s="38" t="s">
         <v>415</v>
       </c>
-      <c r="B243" s="5" t="s">
+      <c r="B247" s="5" t="s">
         <v>417</v>
       </c>
-      <c r="C243" s="5" t="s">
+      <c r="C247" s="5" t="s">
         <v>418</v>
       </c>
-      <c r="D243" s="3" t="s">
+      <c r="D247" s="3" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="244" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A244" s="5" t="s">
+    <row r="248" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A248" s="5" t="s">
         <v>423</v>
       </c>
-      <c r="C244" s="57" t="s">
+      <c r="C248" s="57" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="245" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A245" s="5" t="s">
+    <row r="249" spans="1:22" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A249" s="5" t="s">
         <v>421</v>
       </c>
-      <c r="C245" s="5" t="s">
+      <c r="C249" s="5" t="s">
         <v>422</v>
       </c>
-      <c r="D245" s="3" t="s">
+      <c r="D249" s="3" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A246" s="38" t="s">
+    <row r="250" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A250" s="38" t="s">
         <v>235</v>
       </c>
-      <c r="D246" s="3" t="s">
+      <c r="D250" s="3" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A247" s="38" t="s">
+    <row r="251" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A251" s="38" t="s">
         <v>425</v>
       </c>
-      <c r="D247" s="3" t="s">
+      <c r="D251" s="3" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A248" s="38" t="s">
+    <row r="252" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A252" s="38" t="s">
         <v>427</v>
       </c>
-      <c r="D248" s="3" t="s">
+      <c r="D252" s="3" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A249" s="55" t="s">
+    <row r="253" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A253" s="55" t="s">
         <v>429</v>
-      </c>
-      <c r="B249" s="44"/>
-      <c r="C249" s="44"/>
-      <c r="D249" s="45"/>
-    </row>
-    <row r="250" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A250" s="48"/>
-      <c r="B250" s="58" t="s">
-        <v>437</v>
-      </c>
-      <c r="C250" s="49" t="s">
-        <v>430</v>
-      </c>
-      <c r="D250" s="50"/>
-    </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A251" s="55" t="s">
-        <v>431</v>
-      </c>
-      <c r="B251" s="44"/>
-      <c r="C251" s="44"/>
-      <c r="D251" s="45"/>
-    </row>
-    <row r="252" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A252" s="48"/>
-      <c r="B252" s="49"/>
-      <c r="C252" s="58" t="s">
-        <v>432</v>
-      </c>
-      <c r="D252" s="50"/>
-    </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A253" s="55" t="s">
-        <v>433</v>
       </c>
       <c r="B253" s="44"/>
       <c r="C253" s="44"/>
       <c r="D253" s="45"/>
     </row>
-    <row r="254" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A254" s="46" t="s">
+    <row r="254" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A254" s="48"/>
+      <c r="B254" s="58" t="s">
+        <v>437</v>
+      </c>
+      <c r="C254" s="49" t="s">
+        <v>430</v>
+      </c>
+      <c r="D254" s="50"/>
+    </row>
+    <row r="255" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A255" s="55" t="s">
+        <v>431</v>
+      </c>
+      <c r="B255" s="44"/>
+      <c r="C255" s="44"/>
+      <c r="D255" s="45"/>
+    </row>
+    <row r="256" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A256" s="48"/>
+      <c r="B256" s="49"/>
+      <c r="C256" s="58" t="s">
+        <v>432</v>
+      </c>
+      <c r="D256" s="50"/>
+    </row>
+    <row r="257" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A257" s="55" t="s">
+        <v>433</v>
+      </c>
+      <c r="B257" s="44"/>
+      <c r="C257" s="44"/>
+      <c r="D257" s="45"/>
+    </row>
+    <row r="258" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A258" s="46" t="s">
         <v>435</v>
       </c>
-      <c r="B254" s="57" t="s">
+      <c r="B258" s="57" t="s">
         <v>436</v>
       </c>
-      <c r="C254" s="5" t="s">
+      <c r="C258" s="5" t="s">
         <v>434</v>
       </c>
-      <c r="D254" s="47"/>
-    </row>
-    <row r="255" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A255" s="48"/>
-      <c r="B255" s="49"/>
-      <c r="C255" s="49" t="s">
+      <c r="D258" s="47"/>
+    </row>
+    <row r="259" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A259" s="48"/>
+      <c r="B259" s="49"/>
+      <c r="C259" s="49" t="s">
         <v>438</v>
       </c>
-      <c r="D255" s="50"/>
-    </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A256" s="38" t="s">
+      <c r="D259" s="50"/>
+    </row>
+    <row r="260" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A260" s="38" t="s">
         <v>439</v>
       </c>
-      <c r="B256" s="5" t="s">
+      <c r="B260" s="5" t="s">
         <v>443</v>
       </c>
-      <c r="D256" s="3" t="s">
+      <c r="D260" s="3" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="257" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="B257" s="5" t="s">
+    <row r="261" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B261" s="5" t="s">
         <v>442</v>
       </c>
-      <c r="D257" s="3" t="s">
+      <c r="D261" s="3" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="265" spans="1:22" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A265" s="31"/>
-      <c r="B265" s="32"/>
-      <c r="C265" s="33"/>
-      <c r="D265" s="31"/>
-      <c r="E265" s="34"/>
-      <c r="F265" s="31"/>
-      <c r="G265" s="32"/>
-      <c r="H265" s="31"/>
-      <c r="I265" s="31"/>
-      <c r="J265" s="34"/>
-      <c r="K265" s="31"/>
-      <c r="L265" s="31"/>
-      <c r="M265" s="31"/>
-      <c r="N265" s="31"/>
-      <c r="O265" s="34"/>
-      <c r="P265" s="32"/>
-      <c r="Q265" s="32"/>
-      <c r="R265" s="32"/>
-      <c r="S265" s="32"/>
-      <c r="T265" s="35"/>
-      <c r="U265" s="32"/>
-    </row>
-    <row r="266" spans="1:22" s="36" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A266" s="36" t="s">
+    <row r="269" spans="1:22" s="36" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A269" s="31"/>
+      <c r="B269" s="32"/>
+      <c r="C269" s="33"/>
+      <c r="D269" s="31"/>
+      <c r="E269" s="34"/>
+      <c r="F269" s="31"/>
+      <c r="G269" s="32"/>
+      <c r="H269" s="31"/>
+      <c r="I269" s="31"/>
+      <c r="J269" s="34"/>
+      <c r="K269" s="31"/>
+      <c r="L269" s="31"/>
+      <c r="M269" s="31"/>
+      <c r="N269" s="31"/>
+      <c r="O269" s="34"/>
+      <c r="P269" s="32"/>
+      <c r="Q269" s="32"/>
+      <c r="R269" s="32"/>
+      <c r="S269" s="32"/>
+      <c r="T269" s="35"/>
+      <c r="U269" s="32"/>
+    </row>
+    <row r="270" spans="1:22" s="36" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A270" s="36" t="s">
         <v>489</v>
       </c>
-      <c r="B266" s="37"/>
-      <c r="C266" s="61" t="s">
+      <c r="B270" s="37"/>
+      <c r="C270" s="61" t="s">
         <v>490</v>
       </c>
-      <c r="E266" s="34"/>
-      <c r="G266" s="37"/>
-      <c r="J266" s="34"/>
-      <c r="O266" s="34"/>
-      <c r="Q266" s="37"/>
-      <c r="R266" s="37"/>
-      <c r="T266" s="35"/>
-      <c r="V266" s="37"/>
-    </row>
-    <row r="267" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A267" s="5">
+      <c r="E270" s="34"/>
+      <c r="G270" s="37"/>
+      <c r="J270" s="34"/>
+      <c r="O270" s="34"/>
+      <c r="Q270" s="37"/>
+      <c r="R270" s="37"/>
+      <c r="T270" s="35"/>
+      <c r="V270" s="37"/>
+    </row>
+    <row r="271" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A271" s="5">
         <v>1</v>
       </c>
-      <c r="C267" s="5" t="s">
+      <c r="C271" s="5" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="268" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A268" s="5">
+    <row r="272" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A272" s="5">
         <v>2</v>
       </c>
-      <c r="C268" s="5" t="s">
+      <c r="C272" s="5" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="269" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A269" s="5">
+    <row r="273" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A273" s="5">
         <v>3</v>
       </c>
-      <c r="C269" s="5" t="s">
+      <c r="C273" s="5" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="270" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A270" s="5">
+    <row r="274" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A274" s="5">
         <v>4</v>
       </c>
-      <c r="C270" s="5" t="s">
+      <c r="C274" s="5" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="271" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A271" s="5" t="s">
+    <row r="275" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A275" s="5" t="s">
         <v>495</v>
       </c>
-      <c r="C271" s="5" t="s">
+      <c r="C275" s="5" t="s">
         <v>496</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C56" r:id="rId1" xr:uid="{D4CAF2C4-819C-4857-B4FF-684C5EF88CE2}"/>
-    <hyperlink ref="C66" r:id="rId2" xr:uid="{03454A86-1125-479D-9521-9C049D264793}"/>
+    <hyperlink ref="C60" r:id="rId1" xr:uid="{D4CAF2C4-819C-4857-B4FF-684C5EF88CE2}"/>
+    <hyperlink ref="C70" r:id="rId2" xr:uid="{03454A86-1125-479D-9521-9C049D264793}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="13" fitToHeight="0" orientation="landscape" r:id="rId3"/>

</xml_diff>

<commit_message>
save 19 12 2025
</commit_message>
<xml_diff>
--- a/1 четверть_3_Введение в контроль версий.xlsx
+++ b/1 четверть_3_Введение в контроль версий.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlexServHW\Desktop\GB_Developer_Workbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A08B6EBC-C5CB-4F6D-86A9-4310953B7535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1597E48-2475-41E9-BA9E-FF4A8D8CCD76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3780" yWindow="-17310" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1-3" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="557">
   <si>
     <t>Урок 1</t>
   </si>
@@ -4812,12 +4812,151 @@
 git branch -r - показать локальные ветки удалённого репозитория
 git branch -a - ВСЕ ветки</t>
   </si>
+  <si>
+    <t>git checkout 1.0.0</t>
+  </si>
+  <si>
+    <t>git log --oneline 1.0.0</t>
+  </si>
+  <si>
+    <t>Просмотреть историю до тега</t>
+  </si>
+  <si>
+    <t>Проверить состояние на момент тега</t>
+  </si>
+  <si>
+    <t>git diff 1.0.0 1.1.0</t>
+  </si>
+  <si>
+    <t>Сравнить два тега между собой</t>
+  </si>
+  <si>
+    <t>Подключение по ssh</t>
+  </si>
+  <si>
+    <t>Шаг 1</t>
+  </si>
+  <si>
+    <t># Проверка существующих ключей
+ls -la ~/.ssh/
+# Проверка, что ssh-agent запущен
+eval "$(ssh-agent -s)"
+# Добавьте ключ в ssh-agent
+ssh-add ~/.ssh/id_rsa  # или ваш ключ</t>
+  </si>
+  <si>
+    <t>Подключение при каждой новой сессии работы с удаленным репозиторием github</t>
+  </si>
+  <si>
+    <t>ssh-keygen -t ed25519 -C "your_email@example.com"</t>
+  </si>
+  <si>
+    <t>Ключ будет добавлен в папку ~/.ssh/</t>
+  </si>
+  <si>
+    <t>Нужно добавить ключ в github репозиторий</t>
+  </si>
+  <si>
+    <t>Шаг 2
+Шаг 3</t>
+  </si>
+  <si>
+    <r>
+      <t>cat ~/.ssh/id_ed25519.pub
+Создать файл в ~/.ssh/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">config </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>со следующим содержимым:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Host </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>github-greatnameuser</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+    HostName github.com
+    User git
+    IdentityFile ~/.ssh/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>id_ed25519</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5059,6 +5198,15 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -5510,7 +5658,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2775858</xdr:colOff>
+      <xdr:colOff>2764428</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>2095437</xdr:rowOff>
     </xdr:to>
@@ -5556,7 +5704,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>2350</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>406400</xdr:rowOff>
+      <xdr:rowOff>402590</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5598,9 +5746,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1949711</xdr:colOff>
+      <xdr:colOff>1963046</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>679559</xdr:rowOff>
+      <xdr:rowOff>666224</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5642,9 +5790,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>2202690</xdr:colOff>
+      <xdr:colOff>2189355</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>1415143</xdr:rowOff>
+      <xdr:rowOff>1426573</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5686,7 +5834,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>2341426</xdr:colOff>
+      <xdr:colOff>2345236</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>1143000</xdr:rowOff>
     </xdr:to>
@@ -5730,9 +5878,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>1610591</xdr:colOff>
+      <xdr:colOff>1620116</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>785091</xdr:rowOff>
+      <xdr:rowOff>781281</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5774,7 +5922,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>1989507</xdr:colOff>
+      <xdr:colOff>1997127</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>878744</xdr:rowOff>
     </xdr:to>
@@ -5818,9 +5966,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2676097</xdr:colOff>
+      <xdr:colOff>2683717</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>788311</xdr:rowOff>
+      <xdr:rowOff>784501</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5862,9 +6010,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>1801091</xdr:colOff>
+      <xdr:colOff>1810616</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>806097</xdr:rowOff>
+      <xdr:rowOff>819432</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5906,7 +6054,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1492250</xdr:colOff>
+      <xdr:colOff>1505585</xdr:colOff>
       <xdr:row>43</xdr:row>
       <xdr:rowOff>876885</xdr:rowOff>
     </xdr:to>
@@ -5950,9 +6098,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>3221182</xdr:colOff>
+      <xdr:colOff>3217372</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>655226</xdr:rowOff>
+      <xdr:rowOff>668561</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5994,7 +6142,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>3310150</xdr:colOff>
+      <xdr:colOff>3298720</xdr:colOff>
       <xdr:row>72</xdr:row>
       <xdr:rowOff>378584</xdr:rowOff>
     </xdr:to>
@@ -6084,7 +6232,7 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>3394365</xdr:colOff>
       <xdr:row>76</xdr:row>
-      <xdr:rowOff>556875</xdr:rowOff>
+      <xdr:rowOff>553065</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6126,9 +6274,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>3043646</xdr:colOff>
+      <xdr:colOff>3032216</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>1154546</xdr:rowOff>
+      <xdr:rowOff>1158356</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6170,9 +6318,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>3380442</xdr:colOff>
+      <xdr:colOff>3370917</xdr:colOff>
       <xdr:row>77</xdr:row>
-      <xdr:rowOff>657411</xdr:rowOff>
+      <xdr:rowOff>666936</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6214,9 +6362,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>3309471</xdr:colOff>
+      <xdr:colOff>3298041</xdr:colOff>
       <xdr:row>78</xdr:row>
-      <xdr:rowOff>845831</xdr:rowOff>
+      <xdr:rowOff>853451</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6257,10 +6405,10 @@
       <xdr:rowOff>697311</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>3862613</xdr:colOff>
-      <xdr:row>80</xdr:row>
-      <xdr:rowOff>1647612</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>394</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>2253</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6302,9 +6450,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1415150</xdr:colOff>
+      <xdr:colOff>1426580</xdr:colOff>
       <xdr:row>80</xdr:row>
-      <xdr:rowOff>1015465</xdr:rowOff>
+      <xdr:rowOff>1011655</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6348,7 +6496,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>1563489</xdr:colOff>
       <xdr:row>80</xdr:row>
-      <xdr:rowOff>1163090</xdr:rowOff>
+      <xdr:rowOff>1159280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6390,7 +6538,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1542143</xdr:colOff>
+      <xdr:colOff>1545953</xdr:colOff>
       <xdr:row>80</xdr:row>
       <xdr:rowOff>1561687</xdr:rowOff>
     </xdr:to>
@@ -6468,13 +6616,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>343647</xdr:colOff>
-      <xdr:row>244</xdr:row>
+      <xdr:row>246</xdr:row>
       <xdr:rowOff>622432</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2917952</xdr:colOff>
-      <xdr:row>244</xdr:row>
+      <xdr:colOff>2914142</xdr:colOff>
+      <xdr:row>246</xdr:row>
       <xdr:rowOff>2057948</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -6512,14 +6660,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>358588</xdr:colOff>
-      <xdr:row>247</xdr:row>
+      <xdr:row>249</xdr:row>
       <xdr:rowOff>91490</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2687132</xdr:colOff>
-      <xdr:row>248</xdr:row>
-      <xdr:rowOff>4934</xdr:rowOff>
+      <xdr:colOff>2683322</xdr:colOff>
+      <xdr:row>250</xdr:row>
+      <xdr:rowOff>16364</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6556,14 +6704,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>74706</xdr:colOff>
-      <xdr:row>248</xdr:row>
+      <xdr:row>250</xdr:row>
       <xdr:rowOff>138965</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2756856</xdr:colOff>
-      <xdr:row>248</xdr:row>
-      <xdr:rowOff>1249542</xdr:rowOff>
+      <xdr:colOff>2760666</xdr:colOff>
+      <xdr:row>250</xdr:row>
+      <xdr:rowOff>1241922</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6605,9 +6753,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2265472</xdr:colOff>
+      <xdr:colOff>2269282</xdr:colOff>
       <xdr:row>121</xdr:row>
-      <xdr:rowOff>470085</xdr:rowOff>
+      <xdr:rowOff>473895</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6909,10 +7057,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:X275"/>
+  <dimension ref="A1:X277"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" topLeftCell="A80" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7163,7 +7311,9 @@
         <v>178</v>
       </c>
       <c r="D11" s="25"/>
-      <c r="F11" s="11"/>
+      <c r="F11" s="38" t="s">
+        <v>548</v>
+      </c>
     </row>
     <row r="12" spans="1:24" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
@@ -7178,6 +7328,15 @@
       <c r="D12" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="G12" s="5" t="s">
+        <v>549</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>552</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>553</v>
+      </c>
       <c r="K12" s="5" t="s">
         <v>25</v>
       </c>
@@ -7188,7 +7347,7 @@
         <v>9.0277777777777776E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
@@ -7201,6 +7360,15 @@
       <c r="D13" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="G13" s="5" t="s">
+        <v>555</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>556</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>554</v>
+      </c>
       <c r="K13" s="5" t="s">
         <v>26</v>
       </c>
@@ -7211,12 +7379,18 @@
         <v>9.2361111111111116E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" ht="144" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>20</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>551</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>550</v>
       </c>
       <c r="K14" s="5" t="s">
         <v>511</v>
@@ -7385,7 +7559,7 @@
         <v>3.0902777777777779E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:24" ht="72" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>51</v>
       </c>
@@ -7721,7 +7895,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="45" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:24" ht="72" x14ac:dyDescent="0.3">
       <c r="A45" s="10" t="s">
         <v>108</v>
       </c>
@@ -9298,281 +9472,287 @@
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A215" s="5" t="s">
+        <v>542</v>
+      </c>
       <c r="B215" s="54"/>
+      <c r="C215" s="5" t="s">
+        <v>545</v>
+      </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A216" s="38" t="s">
-        <v>399</v>
-      </c>
-      <c r="D216" s="3" t="s">
-        <v>400</v>
+      <c r="A216" s="5" t="s">
+        <v>543</v>
+      </c>
+      <c r="B216" s="54"/>
+      <c r="C216" s="5" t="s">
+        <v>544</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" s="5" t="s">
-        <v>378</v>
+        <v>546</v>
+      </c>
+      <c r="B217" s="54"/>
+      <c r="C217" s="5" t="s">
+        <v>547</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A218" s="5" t="s">
-        <v>401</v>
+      <c r="A218" s="38" t="s">
+        <v>399</v>
+      </c>
+      <c r="D218" s="3" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" s="5" t="s">
-        <v>402</v>
+        <v>378</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" s="5" t="s">
-        <v>513</v>
+        <v>401</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" s="5" t="s">
-        <v>514</v>
-      </c>
-      <c r="C221" s="5" t="s">
-        <v>516</v>
+        <v>402</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" s="5" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A223" s="5" t="s">
+        <v>514</v>
+      </c>
+      <c r="C223" s="5" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A224" s="5" t="s">
         <v>515</v>
       </c>
-      <c r="C222" s="5" t="s">
+      <c r="C224" s="5" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="225" spans="1:22" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A225" s="31"/>
-      <c r="B225" s="32"/>
-      <c r="C225" s="33"/>
-      <c r="D225" s="31"/>
-      <c r="E225" s="34"/>
-      <c r="F225" s="31"/>
-      <c r="G225" s="32"/>
-      <c r="H225" s="31"/>
-      <c r="I225" s="31"/>
-      <c r="J225" s="34"/>
-      <c r="K225" s="31"/>
-      <c r="L225" s="31"/>
-      <c r="M225" s="31"/>
-      <c r="N225" s="31"/>
-      <c r="O225" s="34"/>
-      <c r="P225" s="32"/>
-      <c r="Q225" s="32"/>
-      <c r="R225" s="32"/>
-      <c r="S225" s="32"/>
-      <c r="T225" s="35"/>
-      <c r="U225" s="32"/>
-    </row>
-    <row r="226" spans="1:22" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A226" s="36" t="s">
+    <row r="227" spans="1:22" s="36" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A227" s="31"/>
+      <c r="B227" s="32"/>
+      <c r="C227" s="33"/>
+      <c r="D227" s="31"/>
+      <c r="E227" s="34"/>
+      <c r="F227" s="31"/>
+      <c r="G227" s="32"/>
+      <c r="H227" s="31"/>
+      <c r="I227" s="31"/>
+      <c r="J227" s="34"/>
+      <c r="K227" s="31"/>
+      <c r="L227" s="31"/>
+      <c r="M227" s="31"/>
+      <c r="N227" s="31"/>
+      <c r="O227" s="34"/>
+      <c r="P227" s="32"/>
+      <c r="Q227" s="32"/>
+      <c r="R227" s="32"/>
+      <c r="S227" s="32"/>
+      <c r="T227" s="35"/>
+      <c r="U227" s="32"/>
+    </row>
+    <row r="228" spans="1:22" s="36" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A228" s="36" t="s">
         <v>478</v>
       </c>
-      <c r="B226" s="37"/>
-      <c r="C226" s="56"/>
-      <c r="E226" s="34"/>
-      <c r="G226" s="37"/>
-      <c r="J226" s="34"/>
-      <c r="O226" s="34"/>
-      <c r="Q226" s="37"/>
-      <c r="R226" s="37"/>
-      <c r="T226" s="35"/>
-      <c r="V226" s="37"/>
-    </row>
-    <row r="227" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A227" s="38" t="s">
-        <v>124</v>
-      </c>
-      <c r="D227" s="3" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="228" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A228" s="5" t="s">
-        <v>480</v>
-      </c>
+      <c r="B228" s="37"/>
+      <c r="C228" s="56"/>
+      <c r="E228" s="34"/>
+      <c r="G228" s="37"/>
+      <c r="J228" s="34"/>
+      <c r="O228" s="34"/>
+      <c r="Q228" s="37"/>
+      <c r="R228" s="37"/>
+      <c r="T228" s="35"/>
+      <c r="V228" s="37"/>
     </row>
     <row r="229" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A229" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="D229" s="3" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="230" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A230" s="5" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="231" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A231" s="38" t="s">
         <v>481</v>
       </c>
-      <c r="C229" s="5" t="s">
+      <c r="C231" s="5" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="230" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="B230" s="5" t="s">
+    <row r="232" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="B232" s="5" t="s">
         <v>457</v>
       </c>
-      <c r="C230" s="5" t="s">
+      <c r="C232" s="5" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="231" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="B231" s="5" t="s">
+    <row r="233" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="B233" s="5" t="s">
         <v>458</v>
       </c>
-      <c r="C231" s="5" t="s">
+      <c r="C233" s="5" t="s">
         <v>484</v>
       </c>
-      <c r="D231" s="3" t="s">
+      <c r="D233" s="3" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="242" spans="1:22" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A242" s="31"/>
-      <c r="B242" s="32"/>
-      <c r="C242" s="33"/>
-      <c r="D242" s="31"/>
-      <c r="E242" s="34"/>
-      <c r="F242" s="31"/>
-      <c r="G242" s="32"/>
-      <c r="H242" s="31"/>
-      <c r="I242" s="31"/>
-      <c r="J242" s="34"/>
-      <c r="K242" s="31"/>
-      <c r="L242" s="31"/>
-      <c r="M242" s="31"/>
-      <c r="N242" s="31"/>
-      <c r="O242" s="34"/>
-      <c r="P242" s="32"/>
-      <c r="Q242" s="32"/>
-      <c r="R242" s="32"/>
-      <c r="S242" s="32"/>
-      <c r="T242" s="35"/>
-      <c r="U242" s="32"/>
-    </row>
-    <row r="243" spans="1:22" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A243" s="36" t="s">
+    <row r="244" spans="1:22" s="36" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A244" s="31"/>
+      <c r="B244" s="32"/>
+      <c r="C244" s="33"/>
+      <c r="D244" s="31"/>
+      <c r="E244" s="34"/>
+      <c r="F244" s="31"/>
+      <c r="G244" s="32"/>
+      <c r="H244" s="31"/>
+      <c r="I244" s="31"/>
+      <c r="J244" s="34"/>
+      <c r="K244" s="31"/>
+      <c r="L244" s="31"/>
+      <c r="M244" s="31"/>
+      <c r="N244" s="31"/>
+      <c r="O244" s="34"/>
+      <c r="P244" s="32"/>
+      <c r="Q244" s="32"/>
+      <c r="R244" s="32"/>
+      <c r="S244" s="32"/>
+      <c r="T244" s="35"/>
+      <c r="U244" s="32"/>
+    </row>
+    <row r="245" spans="1:22" s="36" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A245" s="36" t="s">
         <v>403</v>
       </c>
-      <c r="B243" s="37"/>
-      <c r="C243" s="56" t="s">
+      <c r="B245" s="37"/>
+      <c r="C245" s="56" t="s">
         <v>404</v>
       </c>
-      <c r="E243" s="34"/>
-      <c r="G243" s="37"/>
-      <c r="J243" s="34"/>
-      <c r="O243" s="34"/>
-      <c r="Q243" s="37"/>
-      <c r="R243" s="37"/>
-      <c r="T243" s="35"/>
-      <c r="V243" s="37"/>
-    </row>
-    <row r="244" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A244" s="38" t="s">
+      <c r="E245" s="34"/>
+      <c r="G245" s="37"/>
+      <c r="J245" s="34"/>
+      <c r="O245" s="34"/>
+      <c r="Q245" s="37"/>
+      <c r="R245" s="37"/>
+      <c r="T245" s="35"/>
+      <c r="V245" s="37"/>
+    </row>
+    <row r="246" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A246" s="38" t="s">
         <v>406</v>
       </c>
-      <c r="C244" s="5" t="s">
+      <c r="C246" s="5" t="s">
         <v>409</v>
       </c>
-      <c r="D244" s="3" t="s">
+      <c r="D246" s="3" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="245" spans="1:22" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A245" s="57" t="s">
+    <row r="247" spans="1:22" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A247" s="57" t="s">
         <v>414</v>
       </c>
-      <c r="B245" s="5" t="s">
+      <c r="B247" s="5" t="s">
         <v>408</v>
       </c>
-      <c r="C245" s="57" t="s">
+      <c r="C247" s="57" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="246" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A246" s="5" t="s">
+    <row r="248" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A248" s="5" t="s">
         <v>411</v>
       </c>
-      <c r="C246" s="57" t="s">
+      <c r="C248" s="57" t="s">
         <v>413</v>
       </c>
-      <c r="D246" s="3" t="s">
+      <c r="D248" s="3" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="247" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A247" s="38" t="s">
+    <row r="249" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A249" s="38" t="s">
         <v>415</v>
       </c>
-      <c r="B247" s="5" t="s">
+      <c r="B249" s="5" t="s">
         <v>417</v>
       </c>
-      <c r="C247" s="5" t="s">
+      <c r="C249" s="5" t="s">
         <v>418</v>
       </c>
-      <c r="D247" s="3" t="s">
+      <c r="D249" s="3" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="248" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A248" s="5" t="s">
+    <row r="250" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A250" s="5" t="s">
         <v>423</v>
       </c>
-      <c r="C248" s="57" t="s">
+      <c r="C250" s="57" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="249" spans="1:22" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A249" s="5" t="s">
+    <row r="251" spans="1:22" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A251" s="5" t="s">
         <v>421</v>
       </c>
-      <c r="C249" s="5" t="s">
+      <c r="C251" s="5" t="s">
         <v>422</v>
       </c>
-      <c r="D249" s="3" t="s">
+      <c r="D251" s="3" t="s">
         <v>420</v>
-      </c>
-    </row>
-    <row r="250" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A250" s="38" t="s">
-        <v>235</v>
-      </c>
-      <c r="D250" s="3" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="251" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A251" s="38" t="s">
-        <v>425</v>
-      </c>
-      <c r="D251" s="3" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="252" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A252" s="38" t="s">
+        <v>235</v>
+      </c>
+      <c r="D252" s="3" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="253" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A253" s="38" t="s">
+        <v>425</v>
+      </c>
+      <c r="D253" s="3" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="254" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A254" s="38" t="s">
         <v>427</v>
       </c>
-      <c r="D252" s="3" t="s">
+      <c r="D254" s="3" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="253" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A253" s="55" t="s">
-        <v>429</v>
-      </c>
-      <c r="B253" s="44"/>
-      <c r="C253" s="44"/>
-      <c r="D253" s="45"/>
-    </row>
-    <row r="254" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A254" s="48"/>
-      <c r="B254" s="58" t="s">
-        <v>437</v>
-      </c>
-      <c r="C254" s="49" t="s">
-        <v>430</v>
-      </c>
-      <c r="D254" s="50"/>
     </row>
     <row r="255" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A255" s="55" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B255" s="44"/>
       <c r="C255" s="44"/>
@@ -9580,136 +9760,154 @@
     </row>
     <row r="256" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A256" s="48"/>
-      <c r="B256" s="49"/>
-      <c r="C256" s="58" t="s">
-        <v>432</v>
+      <c r="B256" s="58" t="s">
+        <v>437</v>
+      </c>
+      <c r="C256" s="49" t="s">
+        <v>430</v>
       </c>
       <c r="D256" s="50"/>
     </row>
     <row r="257" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A257" s="55" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B257" s="44"/>
       <c r="C257" s="44"/>
       <c r="D257" s="45"/>
     </row>
-    <row r="258" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A258" s="46" t="s">
+    <row r="258" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A258" s="48"/>
+      <c r="B258" s="49"/>
+      <c r="C258" s="58" t="s">
+        <v>432</v>
+      </c>
+      <c r="D258" s="50"/>
+    </row>
+    <row r="259" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A259" s="55" t="s">
+        <v>433</v>
+      </c>
+      <c r="B259" s="44"/>
+      <c r="C259" s="44"/>
+      <c r="D259" s="45"/>
+    </row>
+    <row r="260" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A260" s="46" t="s">
         <v>435</v>
       </c>
-      <c r="B258" s="57" t="s">
+      <c r="B260" s="57" t="s">
         <v>436</v>
       </c>
-      <c r="C258" s="5" t="s">
+      <c r="C260" s="5" t="s">
         <v>434</v>
       </c>
-      <c r="D258" s="47"/>
-    </row>
-    <row r="259" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A259" s="48"/>
-      <c r="B259" s="49"/>
-      <c r="C259" s="49" t="s">
+      <c r="D260" s="47"/>
+    </row>
+    <row r="261" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A261" s="48"/>
+      <c r="B261" s="49"/>
+      <c r="C261" s="49" t="s">
         <v>438</v>
       </c>
-      <c r="D259" s="50"/>
-    </row>
-    <row r="260" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A260" s="38" t="s">
+      <c r="D261" s="50"/>
+    </row>
+    <row r="262" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A262" s="38" t="s">
         <v>439</v>
       </c>
-      <c r="B260" s="5" t="s">
+      <c r="B262" s="5" t="s">
         <v>443</v>
       </c>
-      <c r="D260" s="3" t="s">
+      <c r="D262" s="3" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="261" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="B261" s="5" t="s">
+    <row r="263" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B263" s="5" t="s">
         <v>442</v>
       </c>
-      <c r="D261" s="3" t="s">
+      <c r="D263" s="3" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="269" spans="1:22" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A269" s="31"/>
-      <c r="B269" s="32"/>
-      <c r="C269" s="33"/>
-      <c r="D269" s="31"/>
-      <c r="E269" s="34"/>
-      <c r="F269" s="31"/>
-      <c r="G269" s="32"/>
-      <c r="H269" s="31"/>
-      <c r="I269" s="31"/>
-      <c r="J269" s="34"/>
-      <c r="K269" s="31"/>
-      <c r="L269" s="31"/>
-      <c r="M269" s="31"/>
-      <c r="N269" s="31"/>
-      <c r="O269" s="34"/>
-      <c r="P269" s="32"/>
-      <c r="Q269" s="32"/>
-      <c r="R269" s="32"/>
-      <c r="S269" s="32"/>
-      <c r="T269" s="35"/>
-      <c r="U269" s="32"/>
-    </row>
-    <row r="270" spans="1:22" s="36" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A270" s="36" t="s">
+    <row r="271" spans="1:22" s="36" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A271" s="31"/>
+      <c r="B271" s="32"/>
+      <c r="C271" s="33"/>
+      <c r="D271" s="31"/>
+      <c r="E271" s="34"/>
+      <c r="F271" s="31"/>
+      <c r="G271" s="32"/>
+      <c r="H271" s="31"/>
+      <c r="I271" s="31"/>
+      <c r="J271" s="34"/>
+      <c r="K271" s="31"/>
+      <c r="L271" s="31"/>
+      <c r="M271" s="31"/>
+      <c r="N271" s="31"/>
+      <c r="O271" s="34"/>
+      <c r="P271" s="32"/>
+      <c r="Q271" s="32"/>
+      <c r="R271" s="32"/>
+      <c r="S271" s="32"/>
+      <c r="T271" s="35"/>
+      <c r="U271" s="32"/>
+    </row>
+    <row r="272" spans="1:22" s="36" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A272" s="36" t="s">
         <v>489</v>
       </c>
-      <c r="B270" s="37"/>
-      <c r="C270" s="61" t="s">
+      <c r="B272" s="37"/>
+      <c r="C272" s="61" t="s">
         <v>490</v>
       </c>
-      <c r="E270" s="34"/>
-      <c r="G270" s="37"/>
-      <c r="J270" s="34"/>
-      <c r="O270" s="34"/>
-      <c r="Q270" s="37"/>
-      <c r="R270" s="37"/>
-      <c r="T270" s="35"/>
-      <c r="V270" s="37"/>
-    </row>
-    <row r="271" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A271" s="5">
+      <c r="E272" s="34"/>
+      <c r="G272" s="37"/>
+      <c r="J272" s="34"/>
+      <c r="O272" s="34"/>
+      <c r="Q272" s="37"/>
+      <c r="R272" s="37"/>
+      <c r="T272" s="35"/>
+      <c r="V272" s="37"/>
+    </row>
+    <row r="273" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A273" s="5">
         <v>1</v>
       </c>
-      <c r="C271" s="5" t="s">
+      <c r="C273" s="5" t="s">
         <v>491</v>
-      </c>
-    </row>
-    <row r="272" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A272" s="5">
-        <v>2</v>
-      </c>
-      <c r="C272" s="5" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="273" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A273" s="5">
-        <v>3</v>
-      </c>
-      <c r="C273" s="5" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="274" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A274" s="5">
+        <v>2</v>
+      </c>
+      <c r="C274" s="5" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A275" s="5">
+        <v>3</v>
+      </c>
+      <c r="C275" s="5" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A276" s="5">
         <v>4</v>
       </c>
-      <c r="C274" s="5" t="s">
+      <c r="C276" s="5" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="275" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A275" s="5" t="s">
+    <row r="277" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A277" s="5" t="s">
         <v>495</v>
       </c>
-      <c r="C275" s="5" t="s">
+      <c r="C277" s="5" t="s">
         <v>496</v>
       </c>
     </row>

</xml_diff>

<commit_message>
save 13 02 2026
</commit_message>
<xml_diff>
--- a/1 четверть_3_Введение в контроль версий.xlsx
+++ b/1 четверть_3_Введение в контроль версий.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlexServHW\Desktop\GB_Developer_Workbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1597E48-2475-41E9-BA9E-FF4A8D8CCD76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2376E424-7969-4726-806F-3CAD709B554B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="-17310" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1-3" sheetId="2" r:id="rId1"/>
@@ -7059,8 +7059,8 @@
   </sheetPr>
   <dimension ref="A1:X277"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B92" sqref="B92"/>
+    <sheetView tabSelected="1" topLeftCell="A206" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B216" sqref="B216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>